<commit_message>
Keywords of Exchange Modulw
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157" count="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157" count="645">
   <si>
     <t>TC_Id</t>
   </si>
@@ -500,6 +500,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -511,6 +512,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -523,6 +525,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -535,6 +538,7 @@
       <sz val="10"/>
       <color rgb="FF2B579A"/>
       <name val="Arial"/>
+      <charset val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -542,6 +546,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -549,6 +554,7 @@
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -603,7 +609,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1177,95 +1183,449 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>123456</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>123456</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>600</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>123456</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>123456</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>600</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1">
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>123456</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5">
+        <v>123456</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1">
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>123456</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>123456</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>600</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>123456</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>123456</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="H7">
+        <v>600</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>123456</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>123456</v>
+      </c>
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="4">
+        <v>45384</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" t="s">
+        <v>29</v>
+      </c>
+      <c r="V8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
Resolved Conflicts of Billing Module
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="162" count="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163" count="1385">
   <si>
     <t>TC_Id</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Mrunal Jagtap</t>
+  </si>
+  <si>
+    <t>458-*+++++</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1773,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1846,8 +1849,11 @@
       <c r="Y10" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+      <c r="Z10">
+        <v>9149212438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -1922,6 +1928,9 @@
       </c>
       <c r="Y11" t="s">
         <v>158</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Added remaining test cases of exchange
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163" count="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166" count="1393">
   <si>
     <t>TC_Id</t>
   </si>
@@ -503,6 +503,15 @@
   </si>
   <si>
     <t>458-*+++++</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>ITi904240046</t>
+  </si>
+  <si>
+    <t>SIsp1021272440268</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1942,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2007,10 +2016,13 @@
         <v>34</v>
       </c>
       <c r="Y12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+        <v>163</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -2084,7 +2096,10 @@
         <v>34</v>
       </c>
       <c r="Y13" t="s">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
test cases from 21 to 40 updated
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -1002,8 +1002,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="G25">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="A46">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1802,7 +1802,6 @@
       <c r="Y10" t="s">
         <v>38</v>
       </c>
-      <c r="Z10"/>
     </row>
     <row r="11" ht="33.75" customHeight="1">
       <c r="A11" t="s">
@@ -4266,7 +4265,7 @@
         <v>82</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="N41" t="s">
         <v>48</v>
@@ -4470,6 +4469,12 @@
       <c r="Y43" t="s">
         <v>38</v>
       </c>
+      <c r="Z43">
+        <v>7719921544</v>
+      </c>
+      <c r="AA43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" t="s">
@@ -4547,6 +4552,12 @@
       <c r="Y44" t="s">
         <v>38</v>
       </c>
+      <c r="Z44">
+        <v>7719921544</v>
+      </c>
+      <c r="AA44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" t="s">
@@ -4624,6 +4635,12 @@
       <c r="Y45" t="s">
         <v>38</v>
       </c>
+      <c r="Z45">
+        <v>7719921544</v>
+      </c>
+      <c r="AA45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" t="s">
@@ -4701,6 +4718,12 @@
       <c r="Y46" t="s">
         <v>38</v>
       </c>
+      <c r="Z46">
+        <v>7719921544</v>
+      </c>
+      <c r="AA46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" t="s">
@@ -4777,6 +4800,12 @@
       </c>
       <c r="Y47" t="s">
         <v>38</v>
+      </c>
+      <c r="Z47">
+        <v>7719921544</v>
+      </c>
+      <c r="AA47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" ht="14.25">

</xml_diff>

<commit_message>
New keywords and Test Cases Added
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -573,7 +573,13 @@
     <t>E_105</t>
   </si>
   <si>
+    <t>Sal</t>
+  </si>
+  <si>
     <t>E_106</t>
+  </si>
+  <si>
+    <t>Sa</t>
   </si>
   <si>
     <t>E_107</t>
@@ -1139,8 +1145,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="T82">
-      <selection activeCell="AB105" sqref="AB105"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="Q85">
+      <selection activeCell="Y108" sqref="Y108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8092,6 +8098,9 @@
       <c r="X99" t="s">
         <v>37</v>
       </c>
+      <c r="Y99" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="100" ht="14.25">
       <c r="A100" t="s">
@@ -8535,15 +8544,15 @@
         <v>37</v>
       </c>
       <c r="Y106" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z106">
-        <v>9149212438</v>
+        <v>45</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>28</v>
@@ -8598,10 +8607,16 @@
       <c r="X107" t="s">
         <v>37</v>
       </c>
+      <c r="Y107" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>28</v>
@@ -8659,7 +8674,7 @@
     </row>
     <row r="109" ht="14.25">
       <c r="A109" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>28</v>
@@ -8717,7 +8732,7 @@
     </row>
     <row r="110" ht="14.25">
       <c r="A110" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>28</v>
@@ -8775,7 +8790,7 @@
     </row>
     <row r="111" ht="14.25">
       <c r="A111" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>28</v>
@@ -8833,7 +8848,7 @@
     </row>
     <row r="112" ht="14.25">
       <c r="A112" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>28</v>
@@ -8891,7 +8906,7 @@
     </row>
     <row r="113" ht="14.25">
       <c r="A113" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>28</v>
@@ -8949,7 +8964,7 @@
     </row>
     <row r="114" ht="14.25">
       <c r="A114" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>28</v>
@@ -9007,7 +9022,7 @@
     </row>
     <row r="115" ht="14.25">
       <c r="A115" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>28</v>
@@ -9065,7 +9080,7 @@
     </row>
     <row r="116" ht="14.25">
       <c r="A116" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>28</v>
@@ -9123,7 +9138,7 @@
     </row>
     <row r="117" ht="14.25">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>28</v>
@@ -9181,7 +9196,7 @@
     </row>
     <row r="118" ht="14.25">
       <c r="A118" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>28</v>
@@ -9239,7 +9254,7 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>28</v>
@@ -9297,7 +9312,7 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>28</v>
@@ -9355,7 +9370,7 @@
     </row>
     <row r="121" ht="14.25">
       <c r="A121" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>28</v>
@@ -9413,7 +9428,7 @@
     </row>
     <row r="122" ht="14.25">
       <c r="A122" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>28</v>
@@ -9471,7 +9486,7 @@
     </row>
     <row r="123" ht="14.25">
       <c r="A123" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>28</v>
@@ -9529,7 +9544,7 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>28</v>
@@ -9587,7 +9602,7 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>28</v>
@@ -9645,7 +9660,7 @@
     </row>
     <row r="126" ht="14.25">
       <c r="A126" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>28</v>
@@ -9703,7 +9718,7 @@
     </row>
     <row r="127" ht="14.25">
       <c r="A127" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>28</v>
@@ -9761,7 +9776,7 @@
     </row>
     <row r="128" ht="14.25">
       <c r="A128" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>28</v>
@@ -9819,7 +9834,7 @@
     </row>
     <row r="129" ht="14.25">
       <c r="A129" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>28</v>
@@ -9877,7 +9892,7 @@
     </row>
     <row r="130" ht="14.25">
       <c r="A130" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>28</v>
@@ -9935,7 +9950,7 @@
     </row>
     <row r="131" ht="14.25">
       <c r="A131" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>28</v>
@@ -9993,7 +10008,7 @@
     </row>
     <row r="132" ht="14.25">
       <c r="A132" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
test case updates 57-67
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -395,10 +395,22 @@
     <t>E_57</t>
   </si>
   <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Sonu nigam</t>
+  </si>
+  <si>
     <t>E_58</t>
   </si>
   <si>
     <t>E_59</t>
+  </si>
+  <si>
+    <t>Alexa : 1</t>
+  </si>
+  <si>
+    <t>Sudhir Phadke</t>
   </si>
   <si>
     <t>E_60</t>
@@ -1002,8 +1014,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="A46">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="Q63">
+      <selection activeCell="Z67" sqref="Z67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5652,12 +5664,18 @@
         <v>37</v>
       </c>
       <c r="Y58" t="s">
-        <v>38</v>
+        <v>125</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>28</v>
@@ -5734,7 +5752,7 @@
     </row>
     <row r="60" ht="14.25">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>28</v>
@@ -5770,7 +5788,7 @@
         <v>67</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="N60" t="s">
         <v>48</v>
@@ -5806,12 +5824,18 @@
         <v>37</v>
       </c>
       <c r="Y60" t="s">
-        <v>38</v>
+        <v>125</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA60">
+        <v>1</v>
       </c>
     </row>
     <row r="61" ht="14.25">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>28</v>
@@ -5847,7 +5871,7 @@
         <v>50</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="N61" t="s">
         <v>48</v>
@@ -5884,11 +5908,17 @@
       </c>
       <c r="Y61" t="s">
         <v>38</v>
+      </c>
+      <c r="Z61">
+        <v>7719921544</v>
+      </c>
+      <c r="AA61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>28</v>
@@ -5924,7 +5954,7 @@
         <v>50</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="N62" t="s">
         <v>48</v>
@@ -5961,11 +5991,17 @@
       </c>
       <c r="Y62" t="s">
         <v>38</v>
+      </c>
+      <c r="Z62">
+        <v>7719921544</v>
+      </c>
+      <c r="AA62">
+        <v>1</v>
       </c>
     </row>
     <row r="63" ht="14.25">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>28</v>
@@ -6038,11 +6074,17 @@
       </c>
       <c r="Y63" t="s">
         <v>38</v>
+      </c>
+      <c r="Z63">
+        <v>7719921544</v>
+      </c>
+      <c r="AA63">
+        <v>1</v>
       </c>
     </row>
     <row r="64" ht="14.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>28</v>
@@ -6115,11 +6157,17 @@
       </c>
       <c r="Y64" t="s">
         <v>38</v>
+      </c>
+      <c r="Z64">
+        <v>7719921544</v>
+      </c>
+      <c r="AA64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>28</v>
@@ -6192,11 +6240,17 @@
       </c>
       <c r="Y65" t="s">
         <v>38</v>
+      </c>
+      <c r="Z65">
+        <v>7719921544</v>
+      </c>
+      <c r="AA65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>28</v>
@@ -6269,11 +6323,17 @@
       </c>
       <c r="Y66" t="s">
         <v>38</v>
+      </c>
+      <c r="Z66">
+        <v>7719921544</v>
+      </c>
+      <c r="AA66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>28</v>
@@ -6346,11 +6406,17 @@
       </c>
       <c r="Y67" t="s">
         <v>38</v>
+      </c>
+      <c r="Z67">
+        <v>7719921544</v>
+      </c>
+      <c r="AA67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>28</v>
@@ -6427,7 +6493,7 @@
     </row>
     <row r="69" ht="14.25">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>28</v>
@@ -6504,7 +6570,7 @@
     </row>
     <row r="70" ht="14.25">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>28</v>
@@ -6581,7 +6647,7 @@
     </row>
     <row r="71" ht="14.25">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>28</v>
@@ -6658,7 +6724,7 @@
     </row>
     <row r="72" ht="14.25">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>28</v>
@@ -6735,7 +6801,7 @@
     </row>
     <row r="73" ht="14.25">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>28</v>
@@ -6812,7 +6878,7 @@
     </row>
     <row r="74" ht="14.25">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -6828,7 +6894,7 @@
     </row>
     <row r="75" ht="14.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -6844,7 +6910,7 @@
     </row>
     <row r="76" ht="14.25">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -6860,7 +6926,7 @@
     </row>
     <row r="77" ht="14.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -6876,7 +6942,7 @@
     </row>
     <row r="78" ht="14.25">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -6892,7 +6958,7 @@
     </row>
     <row r="79" ht="14.25">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -6908,7 +6974,7 @@
     </row>
     <row r="80" ht="14.25">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -6924,7 +6990,7 @@
     </row>
     <row r="81" ht="14.25">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -6940,7 +7006,7 @@
     </row>
     <row r="82" ht="14.25">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -6956,7 +7022,7 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -6972,72 +7038,72 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -7047,7 +7113,7 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -7057,7 +7123,7 @@
     </row>
     <row r="99" ht="33" customHeight="1">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -7067,7 +7133,7 @@
     </row>
     <row r="100" ht="34.8" customHeight="1">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>

</xml_diff>

<commit_message>
TC 50 to 53
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="160">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -316,94 +316,79 @@
     <t xml:space="preserve">E_49</t>
   </si>
   <si>
+    <t xml:space="preserve">somesh wankhade</t>
+  </si>
+  <si>
     <t xml:space="preserve">E_50</t>
   </si>
   <si>
-    <t xml:space="preserve">Null</t>
+    <t xml:space="preserve">E_51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIi911197240001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash : 149, paytm : 149, on-account : 252</t>
   </si>
   <si>
     <t xml:space="preserve">8906118410781: 4</t>
   </si>
   <si>
-    <t xml:space="preserve">list : Assortment_Item</t>
+    <t xml:space="preserve">E_58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash : 275, paytm : 275, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paytm : 200, card : 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Rupees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash : 200, card : 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8906118412761 : 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash : 100, paytm : 100, voucher : 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list : Bill_Level</t>
   </si>
   <si>
     <t xml:space="preserve">Amount : 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 100, paytm : 100, voucher : 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on-account : 550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 100, on-account : 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Specificqty-Flat-rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 298 , on-account : 252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paytm : 298, on-account : 252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on-account : 252 , card: 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 149, paytm : 149, on-account : 252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 275, paytm : 275, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paytm : 200, card : 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBSB-Any Qty-get pool-spf-Rupees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 200, card : 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118412761 : 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list : Bill_Level</t>
   </si>
   <si>
     <t xml:space="preserve">E_62</t>
@@ -804,8 +789,8 @@
   </sheetPr>
   <dimension ref="A1:AMF92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA50" activeCellId="0" sqref="AA50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y53" activeCellId="0" sqref="Y53:Z53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,11 +802,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="41.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="21" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.54"/>
@@ -4594,6 +4579,15 @@
       <c r="X48" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="Y48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA48" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -4668,6 +4662,15 @@
       <c r="X49" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="Y49" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA49" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -4745,8 +4748,8 @@
       <c r="Y50" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Z50" s="3" t="s">
-        <v>89</v>
+      <c r="Z50" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="AA50" s="0" t="n">
         <v>1</v>
@@ -4754,24 +4757,24 @@
     </row>
     <row r="51" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F51" s="2" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G51" s="1" t="n">
+      <c r="F51" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="H51" s="0" t="n">
@@ -4780,40 +4783,40 @@
       <c r="I51" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J51" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K51" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L51" s="0" t="s">
-        <v>99</v>
+      <c r="J51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N51" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="O51" s="4" t="n">
         <v>45384</v>
       </c>
-      <c r="P51" s="4" t="s">
+      <c r="P51" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q51" s="4" t="s">
+      <c r="Q51" s="5" t="s">
         <v>36</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="T51" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="U51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U51" s="0" t="s">
         <v>33</v>
       </c>
       <c r="V51" s="0" t="s">
@@ -4822,24 +4825,36 @@
       <c r="W51" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="X51" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z51" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA51" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F52" s="2" t="n">
+      <c r="F52" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G52" s="0" t="n">
@@ -4851,32 +4866,32 @@
       <c r="I52" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J52" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K52" s="10" t="n">
-        <v>1</v>
+      <c r="J52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N52" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="O52" s="4" t="n">
         <v>45384</v>
       </c>
-      <c r="P52" s="4" t="s">
+      <c r="P52" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q52" s="4" t="s">
+      <c r="Q52" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R52" s="11" t="n">
-        <v>7709577438</v>
+      <c r="R52" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S52" s="1" t="s">
         <v>33</v>
@@ -4884,7 +4899,7 @@
       <c r="T52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U52" s="1" t="s">
+      <c r="U52" s="0" t="s">
         <v>33</v>
       </c>
       <c r="V52" s="0" t="s">
@@ -4893,24 +4908,36 @@
       <c r="W52" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="X52" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z52" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA52" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D53" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F53" s="2" t="n">
+      <c r="F53" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G53" s="0" t="n">
@@ -4922,32 +4949,32 @@
       <c r="I53" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J53" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K53" s="10" t="n">
-        <v>1</v>
+      <c r="J53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N53" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="O53" s="4" t="n">
         <v>45384</v>
       </c>
-      <c r="P53" s="4" t="s">
+      <c r="P53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q53" s="4" t="s">
+      <c r="Q53" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R53" s="11" t="n">
-        <v>7709577438</v>
+      <c r="R53" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>33</v>
@@ -4955,7 +4982,7 @@
       <c r="T53" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U53" s="1" t="s">
+      <c r="U53" s="0" t="s">
         <v>33</v>
       </c>
       <c r="V53" s="0" t="s">
@@ -4964,24 +4991,36 @@
       <c r="W53" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="X53" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z53" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA53" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="6" t="n">
+      <c r="D54" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="6" t="n">
+      <c r="F54" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G54" s="0" t="n">
@@ -4990,22 +5029,22 @@
       <c r="H54" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="I54" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J54" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K54" s="8" t="n">
-        <v>1</v>
+      <c r="J54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="M54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N54" s="8" t="s">
+      <c r="N54" s="0" t="s">
         <v>33</v>
       </c>
       <c r="O54" s="4" t="n">
@@ -5026,33 +5065,45 @@
       <c r="T54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V54" s="8" t="s">
+      <c r="U54" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V54" s="0" t="s">
         <v>37</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="X54" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z54" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA54" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="2" t="n">
+      <c r="D55" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F55" s="6" t="n">
+      <c r="F55" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G55" s="0" t="n">
@@ -5061,22 +5112,22 @@
       <c r="H55" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J55" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K55" s="8" t="n">
-        <v>1</v>
+      <c r="J55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N55" s="8" t="s">
+      <c r="N55" s="0" t="s">
         <v>33</v>
       </c>
       <c r="O55" s="4" t="n">
@@ -5097,33 +5148,36 @@
       <c r="T55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U55" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V55" s="8" t="s">
+      <c r="U55" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="V55" s="0" t="s">
         <v>37</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="X55" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D56" s="2" t="n">
+      <c r="D56" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="2" t="n">
+      <c r="F56" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G56" s="0" t="n">
@@ -5132,35 +5186,35 @@
       <c r="H56" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="I56" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J56" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K56" s="10" t="n">
-        <v>1</v>
+      <c r="J56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N56" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="O56" s="4" t="n">
         <v>45384</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="P56" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q56" s="4" t="s">
+      <c r="Q56" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R56" s="11" t="n">
-        <v>7709577438</v>
+      <c r="R56" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S56" s="1" t="s">
         <v>33</v>
@@ -5168,7 +5222,7 @@
       <c r="T56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U56" s="1" t="s">
+      <c r="U56" s="0" t="s">
         <v>33</v>
       </c>
       <c r="V56" s="0" t="s">
@@ -5177,24 +5231,27 @@
       <c r="W56" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="X56" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="G57" s="0" t="n">
@@ -5203,35 +5260,35 @@
       <c r="H57" s="0" t="n">
         <v>600</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="I57" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J57" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K57" s="10" t="n">
-        <v>1</v>
+      <c r="J57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N57" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="O57" s="4" t="n">
         <v>45384</v>
       </c>
-      <c r="P57" s="4" t="s">
+      <c r="P57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q57" s="4" t="s">
+      <c r="Q57" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R57" s="11" t="n">
-        <v>7709577438</v>
+      <c r="R57" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S57" s="1" t="s">
         <v>33</v>
@@ -5239,7 +5296,7 @@
       <c r="T57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U57" s="1" t="s">
+      <c r="U57" s="0" t="s">
         <v>33</v>
       </c>
       <c r="V57" s="0" t="s">
@@ -5248,10 +5305,13 @@
       <c r="W57" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="X57" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>29</v>
@@ -5284,13 +5344,13 @@
         <v>1</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O58" s="4" t="n">
         <v>45384</v>
@@ -5322,7 +5382,7 @@
     </row>
     <row r="59" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>29</v>
@@ -5355,13 +5415,13 @@
         <v>1</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O59" s="4" t="n">
         <v>45384</v>
@@ -5393,7 +5453,7 @@
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>29</v>
@@ -5426,13 +5486,13 @@
         <v>1</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O60" s="4" t="n">
         <v>45384</v>
@@ -5464,7 +5524,7 @@
     </row>
     <row r="61" s="8" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>29</v>
@@ -5491,19 +5551,19 @@
         <v>32</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="K61" s="8" t="n">
         <v>1</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>34</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O61" s="13" t="n">
         <v>45384</v>
@@ -6005,7 +6065,7 @@
     </row>
     <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>29</v>
@@ -6038,13 +6098,13 @@
         <v>1</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O62" s="4" t="n">
         <v>45384</v>
@@ -6059,10 +6119,10 @@
         <v>7709577438</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="T62" s="1" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="U62" s="1" t="s">
         <v>33</v>
@@ -6076,7 +6136,7 @@
     </row>
     <row r="63" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>29</v>
@@ -6109,7 +6169,7 @@
         <v>33</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>34</v>
@@ -6147,7 +6207,7 @@
     </row>
     <row r="64" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>29</v>
@@ -6174,7 +6234,7 @@
         <v>32</v>
       </c>
       <c r="J64" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K64" s="8" t="n">
         <v>1</v>
@@ -6213,12 +6273,12 @@
         <v>37</v>
       </c>
       <c r="W64" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>29</v>
@@ -6251,7 +6311,7 @@
         <v>33</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>34</v>
@@ -6284,12 +6344,12 @@
         <v>37</v>
       </c>
       <c r="W65" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>29</v>
@@ -6322,7 +6382,7 @@
         <v>33</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>34</v>
@@ -6355,12 +6415,12 @@
         <v>37</v>
       </c>
       <c r="W66" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>29</v>
@@ -6393,13 +6453,13 @@
         <v>1</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O67" s="4" t="n">
         <v>45384</v>
@@ -6426,12 +6486,12 @@
         <v>37</v>
       </c>
       <c r="W67" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>29</v>
@@ -6464,13 +6524,13 @@
         <v>1</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O68" s="4" t="n">
         <v>45384</v>
@@ -6497,12 +6557,12 @@
         <v>37</v>
       </c>
       <c r="W68" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>29</v>
@@ -6535,13 +6595,13 @@
         <v>1</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O69" s="4" t="n">
         <v>45384</v>
@@ -6573,7 +6633,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>29</v>
@@ -6606,13 +6666,13 @@
         <v>1</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N70" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O70" s="4" t="n">
         <v>45384</v>
@@ -6644,7 +6704,7 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>29</v>
@@ -6677,13 +6737,13 @@
         <v>1</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N71" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O71" s="4" t="n">
         <v>45384</v>
@@ -6715,7 +6775,7 @@
     </row>
     <row r="72" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>29</v>
@@ -6748,13 +6808,13 @@
         <v>1</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N72" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O72" s="4" t="n">
         <v>45384</v>
@@ -6786,7 +6846,7 @@
     </row>
     <row r="73" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>29</v>
@@ -6819,13 +6879,13 @@
         <v>1</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M73" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N73" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O73" s="4" t="n">
         <v>45384</v>
@@ -6840,7 +6900,7 @@
         <v>7709577438</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="T73" s="1" t="s">
         <v>33</v>
@@ -6857,7 +6917,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -6873,7 +6933,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -6889,7 +6949,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -6905,7 +6965,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -6921,7 +6981,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -6937,7 +6997,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -6953,7 +7013,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -6969,7 +7029,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -6985,7 +7045,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -7001,7 +7061,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -7017,47 +7077,47 @@
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new testcases and keywords
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Calc"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mrunal\PycharmProjects\Zwing QA Automation\zwing-qa-automation\TestData\Web_POS\Exchange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anand\PycharmProjects\Zwing QA Automation\zwing-qa-automation\TestData\Web_POS\Exchange\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1082,8 +1082,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="H52">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="A55">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2213,10 +2213,10 @@
         <v>38</v>
       </c>
       <c r="Y13" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z13" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>33</v>
@@ -2301,8 +2301,8 @@
       <c r="Y14" t="s">
         <v>49</v>
       </c>
-      <c r="Z14" s="8">
-        <v>9149212438</v>
+      <c r="Z14" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA14" s="8" t="s">
         <v>33</v>
@@ -2387,8 +2387,8 @@
       <c r="Y15" t="s">
         <v>49</v>
       </c>
-      <c r="Z15" s="8">
-        <v>9149212438</v>
+      <c r="Z15" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA15">
         <v>1</v>
@@ -2473,8 +2473,8 @@
       <c r="Y16" t="s">
         <v>49</v>
       </c>
-      <c r="Z16" s="8">
-        <v>9149212438</v>
+      <c r="Z16" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA16">
         <v>1</v>
@@ -2559,8 +2559,8 @@
       <c r="Y17" t="s">
         <v>49</v>
       </c>
-      <c r="Z17" s="8">
-        <v>9149212438</v>
+      <c r="Z17" s="5">
+        <v>7709577438</v>
       </c>
       <c r="AA17" s="8" t="s">
         <v>33</v>
@@ -7217,8 +7217,8 @@
       <c r="Y72" t="s">
         <v>49</v>
       </c>
-      <c r="Z72" s="8">
-        <v>9149212438</v>
+      <c r="Z72" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA72">
         <v>1</v>
@@ -7283,7 +7283,7 @@
         <v>7709577438</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="T73" s="2" t="s">
         <v>33</v>
@@ -7303,8 +7303,8 @@
       <c r="Y73" t="s">
         <v>49</v>
       </c>
-      <c r="Z73" s="8">
-        <v>9149212438</v>
+      <c r="Z73" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA73">
         <v>1</v>
@@ -7369,7 +7369,7 @@
         <v>7709577438</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="T74" s="2" t="s">
         <v>33</v>
@@ -7389,8 +7389,8 @@
       <c r="Y74" t="s">
         <v>49</v>
       </c>
-      <c r="Z74" s="8">
-        <v>9149212438</v>
+      <c r="Z74" s="5">
+        <v>9595952595</v>
       </c>
       <c r="AA74">
         <v>1</v>

</xml_diff>

<commit_message>
TC 55 and 56
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="161">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t xml:space="preserve">E_56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624cuS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarak mehta</t>
   </si>
   <si>
     <t xml:space="preserve">E_57</t>
@@ -783,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:AMF92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W39" activeCellId="1" sqref="Y52:Z52 W39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S34" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X56" activeCellId="0" sqref="X56:AA56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5154,6 +5163,15 @@
       <c r="X55" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="Y55" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z55" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA55" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -5228,13 +5246,22 @@
       <c r="X56" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="Y56" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA56" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>29</v>
+      <c r="B57" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>30</v>
@@ -5243,7 +5270,7 @@
         <v>123456</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>123456</v>
@@ -5302,10 +5329,19 @@
       <c r="X57" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="Y57" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z57" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA57" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>29</v>
@@ -5338,13 +5374,13 @@
         <v>1</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O58" s="4" t="n">
         <v>45384</v>
@@ -5376,7 +5412,7 @@
     </row>
     <row r="59" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>29</v>
@@ -5409,13 +5445,13 @@
         <v>1</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O59" s="4" t="n">
         <v>45384</v>
@@ -5447,7 +5483,7 @@
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>29</v>
@@ -5480,13 +5516,13 @@
         <v>1</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O60" s="4" t="n">
         <v>45384</v>
@@ -5518,7 +5554,7 @@
     </row>
     <row r="61" s="8" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>29</v>
@@ -5545,19 +5581,19 @@
         <v>32</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K61" s="8" t="n">
         <v>1</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>34</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="O61" s="13" t="n">
         <v>45384</v>
@@ -6059,7 +6095,7 @@
     </row>
     <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>29</v>
@@ -6092,13 +6128,13 @@
         <v>1</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O62" s="4" t="n">
         <v>45384</v>
@@ -6113,10 +6149,10 @@
         <v>7709577438</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="T62" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="U62" s="1" t="s">
         <v>33</v>
@@ -6130,7 +6166,7 @@
     </row>
     <row r="63" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>29</v>
@@ -6163,7 +6199,7 @@
         <v>33</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>34</v>
@@ -6201,7 +6237,7 @@
     </row>
     <row r="64" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>29</v>
@@ -6228,7 +6264,7 @@
         <v>32</v>
       </c>
       <c r="J64" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K64" s="8" t="n">
         <v>1</v>
@@ -6267,12 +6303,12 @@
         <v>37</v>
       </c>
       <c r="W64" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>29</v>
@@ -6305,7 +6341,7 @@
         <v>33</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>34</v>
@@ -6338,12 +6374,12 @@
         <v>37</v>
       </c>
       <c r="W65" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>29</v>
@@ -6376,7 +6412,7 @@
         <v>33</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>34</v>
@@ -6409,12 +6445,12 @@
         <v>37</v>
       </c>
       <c r="W66" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>29</v>
@@ -6447,13 +6483,13 @@
         <v>1</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O67" s="4" t="n">
         <v>45384</v>
@@ -6480,12 +6516,12 @@
         <v>37</v>
       </c>
       <c r="W67" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>29</v>
@@ -6518,13 +6554,13 @@
         <v>1</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N68" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O68" s="4" t="n">
         <v>45384</v>
@@ -6551,12 +6587,12 @@
         <v>37</v>
       </c>
       <c r="W68" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>29</v>
@@ -6589,13 +6625,13 @@
         <v>1</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O69" s="4" t="n">
         <v>45384</v>
@@ -6627,7 +6663,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>29</v>
@@ -6660,13 +6696,13 @@
         <v>1</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N70" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O70" s="4" t="n">
         <v>45384</v>
@@ -6698,7 +6734,7 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>29</v>
@@ -6731,13 +6767,13 @@
         <v>1</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N71" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O71" s="4" t="n">
         <v>45384</v>
@@ -6769,7 +6805,7 @@
     </row>
     <row r="72" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>29</v>
@@ -6802,13 +6838,13 @@
         <v>1</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N72" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O72" s="4" t="n">
         <v>45384</v>
@@ -6840,7 +6876,7 @@
     </row>
     <row r="73" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>29</v>
@@ -6873,13 +6909,13 @@
         <v>1</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M73" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N73" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O73" s="4" t="n">
         <v>45384</v>
@@ -6894,7 +6930,7 @@
         <v>7709577438</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="T73" s="1" t="s">
         <v>33</v>
@@ -6911,7 +6947,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -6927,7 +6963,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -6943,7 +6979,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -6959,7 +6995,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -6975,7 +7011,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -6991,7 +7027,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -7007,7 +7043,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -7023,7 +7059,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -7039,7 +7075,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -7055,7 +7091,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -7071,47 +7107,47 @@
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test cases and keywords
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -581,10 +581,7 @@
     <t>cash : 100, paytm : 100, voucher : 8</t>
   </si>
   <si>
-    <t>8906118410781 : 9</t>
-  </si>
-  <si>
-    <t>8906118410781: 12</t>
+    <t>Alexa67 : 2</t>
   </si>
   <si>
     <t>E_81</t>
@@ -1342,8 +1339,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="L58">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="K55">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1462,7 +1459,6 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AO1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s">
@@ -8350,7 +8346,6 @@
       <c r="AD77" t="s">
         <v>175</v>
       </c>
-      <c r="AE77"/>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" t="s">
@@ -8590,7 +8585,7 @@
         <v>38</v>
       </c>
       <c r="R80" s="11">
-        <v>7709577438</v>
+        <v>8080808080</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>82</v>
@@ -8663,11 +8658,11 @@
       <c r="L81" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="M81" t="s">
         <v>187</v>
       </c>
       <c r="N81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O81" s="10">
         <v>45384</v>
@@ -8679,7 +8674,7 @@
         <v>38</v>
       </c>
       <c r="R81" s="11">
-        <v>7709577438</v>
+        <v>3030303030</v>
       </c>
       <c r="S81" s="2" t="s">
         <v>82</v>
@@ -8713,11 +8708,14 @@
       </c>
       <c r="AC81" s="8" t="s">
         <v>35</v>
+      </c>
+      <c r="AD81" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="82" ht="14.25">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>31</v>
@@ -8742,7 +8740,7 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>31</v>
@@ -8767,7 +8765,7 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>31</v>
@@ -8784,7 +8782,7 @@
     </row>
     <row r="85" ht="14.25">
       <c r="A85" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>31</v>
@@ -8801,7 +8799,7 @@
     </row>
     <row r="86" ht="14.25">
       <c r="A86" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>31</v>
@@ -8818,7 +8816,7 @@
     </row>
     <row r="87" ht="14.25">
       <c r="A87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>31</v>
@@ -8835,7 +8833,7 @@
     </row>
     <row r="88" ht="14.25">
       <c r="A88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>31</v>
@@ -8852,7 +8850,7 @@
     </row>
     <row r="89" ht="14.25">
       <c r="A89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>31</v>
@@ -8869,7 +8867,7 @@
     </row>
     <row r="90" ht="14.25">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>31</v>
@@ -8886,7 +8884,7 @@
     </row>
     <row r="91" ht="14.25">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>31</v>
@@ -8903,7 +8901,7 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>31</v>
@@ -8920,10 +8918,10 @@
     </row>
     <row r="93" ht="14.25">
       <c r="A93" t="s">
+        <v>199</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>32</v>
@@ -9009,10 +9007,10 @@
     </row>
     <row r="94" ht="14.25">
       <c r="A94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>32</v>
@@ -9098,10 +9096,10 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>32</v>
@@ -9187,10 +9185,10 @@
     </row>
     <row r="96" ht="14.25">
       <c r="A96" t="s">
+        <v>203</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>205</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>32</v>
@@ -9199,7 +9197,7 @@
         <v>123456</v>
       </c>
       <c r="E96" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F96" s="4">
         <v>123456</v>
@@ -9276,10 +9274,10 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>32</v>
@@ -9365,10 +9363,10 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>32</v>
@@ -9454,10 +9452,10 @@
     </row>
     <row r="99" ht="33" customHeight="1">
       <c r="A99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>32</v>
@@ -9540,10 +9538,10 @@
     </row>
     <row r="100" ht="34.8" customHeight="1">
       <c r="A100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>32</v>
@@ -9615,7 +9613,7 @@
         <v>48</v>
       </c>
       <c r="Z100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA100" s="5" t="s">
         <v>35</v>
@@ -9629,10 +9627,10 @@
     </row>
     <row r="101" ht="33.75" customHeight="1">
       <c r="A101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>32</v>
@@ -9704,7 +9702,7 @@
         <v>51</v>
       </c>
       <c r="Z101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AA101" s="5" t="s">
         <v>35</v>
@@ -9718,10 +9716,10 @@
     </row>
     <row r="102" ht="33.75" customHeight="1">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>32</v>
@@ -9807,10 +9805,10 @@
     </row>
     <row r="103" ht="33.75" customHeight="1">
       <c r="A103" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>32</v>
@@ -9896,10 +9894,10 @@
     </row>
     <row r="104" ht="33.75" customHeight="1">
       <c r="A104" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>32</v>
@@ -9985,10 +9983,10 @@
     </row>
     <row r="105" ht="33.75" customHeight="1">
       <c r="A105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>32</v>
@@ -10074,10 +10072,10 @@
     </row>
     <row r="106" ht="18" customHeight="1">
       <c r="A106" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>32</v>
@@ -10149,7 +10147,7 @@
         <v>48</v>
       </c>
       <c r="Z106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA106" s="5" t="s">
         <v>35</v>
@@ -10163,10 +10161,10 @@
     </row>
     <row r="107" ht="19.5" customHeight="1">
       <c r="A107" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>32</v>
@@ -10238,7 +10236,7 @@
         <v>48</v>
       </c>
       <c r="Z107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AA107" s="5" t="s">
         <v>35</v>
@@ -10252,10 +10250,10 @@
     </row>
     <row r="108" ht="30" customHeight="1">
       <c r="A108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>32</v>
@@ -10341,10 +10339,10 @@
     </row>
     <row r="109" ht="26.25" customHeight="1">
       <c r="A109" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>32</v>
@@ -10430,10 +10428,10 @@
     </row>
     <row r="110" ht="30" customHeight="1">
       <c r="A110" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>32</v>
@@ -10519,10 +10517,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="14.25">
       <c r="A111" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>32</v>
@@ -26955,10 +26953,10 @@
     </row>
     <row r="112" ht="31.5" customHeight="1">
       <c r="A112" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>32</v>
@@ -27044,10 +27042,10 @@
     </row>
     <row r="113" ht="31.5" customHeight="1">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>32</v>
@@ -27133,10 +27131,10 @@
     </row>
     <row r="114" ht="31.5" customHeight="1">
       <c r="A114" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>32</v>
@@ -27222,10 +27220,10 @@
     </row>
     <row r="115" ht="31.5" customHeight="1">
       <c r="A115" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>32</v>
@@ -27311,10 +27309,10 @@
     </row>
     <row r="116" ht="31.5" customHeight="1">
       <c r="A116" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>32</v>
@@ -27400,10 +27398,10 @@
     </row>
     <row r="117" ht="32.25" customHeight="1">
       <c r="A117" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>32</v>
@@ -27489,10 +27487,10 @@
     </row>
     <row r="118" ht="28.5" customHeight="1">
       <c r="A118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>32</v>
@@ -27578,10 +27576,10 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>233</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>32</v>
@@ -27590,7 +27588,7 @@
         <v>123456</v>
       </c>
       <c r="E119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F119" s="4">
         <v>123456</v>
@@ -27667,10 +27665,10 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>32</v>
@@ -27756,10 +27754,10 @@
     </row>
     <row r="121" ht="14.25">
       <c r="A121" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>32</v>
@@ -27845,10 +27843,10 @@
     </row>
     <row r="122" ht="14.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>32</v>
@@ -27934,10 +27932,10 @@
     </row>
     <row r="123" ht="14.25">
       <c r="A123" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>32</v>
@@ -28023,10 +28021,10 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>32</v>
@@ -28112,10 +28110,10 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>32</v>
@@ -28201,10 +28199,10 @@
     </row>
     <row r="126" ht="14.25">
       <c r="A126" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>32</v>
@@ -28290,10 +28288,10 @@
     </row>
     <row r="127" ht="14.25">
       <c r="A127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>32</v>
@@ -28379,10 +28377,10 @@
     </row>
     <row r="128" ht="14.25">
       <c r="A128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>32</v>
@@ -28468,10 +28466,10 @@
     </row>
     <row r="129" ht="14.25">
       <c r="A129" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>32</v>
@@ -28557,10 +28555,10 @@
     </row>
     <row r="130" ht="14.25">
       <c r="A130" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>32</v>
@@ -28646,10 +28644,10 @@
     </row>
     <row r="131" ht="14.25">
       <c r="A131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>32</v>
@@ -28735,10 +28733,10 @@
     </row>
     <row r="132" ht="14.25">
       <c r="A132" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>32</v>
@@ -28824,82 +28822,82 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug tag removal and checkout keyword modify
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="290">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -374,6 +374,9 @@
       </rPr>
       <t xml:space="preserve"> : 1</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sarvesh nikumbh</t>
   </si>
   <si>
     <t xml:space="preserve">E_46</t>
@@ -1061,7 +1064,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1144,42 +1147,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1440,10 +1407,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ148"/>
+  <dimension ref="A1:AH148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M50" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M86" activeCellId="0" sqref="M86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S20" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA47" activeCellId="0" sqref="AA47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6077,13 +6044,13 @@
         <v>44</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z46" s="4" t="n">
-        <v>5555555555</v>
+        <v>52</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="AA46" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB46" s="8" t="s">
         <v>39</v>
@@ -6106,7 +6073,7 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>35</v>
@@ -6142,7 +6109,7 @@
         <v>39</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>39</v>
@@ -6181,7 +6148,7 @@
         <v>52</v>
       </c>
       <c r="Z47" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AA47" s="4" t="n">
         <v>3</v>
@@ -6207,7 +6174,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>35</v>
@@ -6282,7 +6249,7 @@
         <v>52</v>
       </c>
       <c r="Z48" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AA48" s="4" t="n">
         <v>4</v>
@@ -6308,7 +6275,7 @@
     </row>
     <row r="49" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>35</v>
@@ -6335,7 +6302,7 @@
         <v>38</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K49" s="15" t="n">
         <v>1</v>
@@ -6383,7 +6350,7 @@
         <v>52</v>
       </c>
       <c r="Z49" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AA49" s="4" t="n">
         <v>1</v>
@@ -6409,7 +6376,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>35</v>
@@ -6484,7 +6451,7 @@
         <v>52</v>
       </c>
       <c r="Z50" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AA50" s="4" t="n">
         <v>1</v>
@@ -6510,7 +6477,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>35</v>
@@ -6585,7 +6552,7 @@
         <v>52</v>
       </c>
       <c r="Z51" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AA51" s="4" t="n">
         <v>1</v>
@@ -6611,7 +6578,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>35</v>
@@ -6686,7 +6653,7 @@
         <v>52</v>
       </c>
       <c r="Z52" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AA52" s="4" t="n">
         <v>1</v>
@@ -6712,7 +6679,7 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>35</v>
@@ -6787,7 +6754,7 @@
         <v>52</v>
       </c>
       <c r="Z53" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AA53" s="4" t="n">
         <v>3</v>
@@ -6813,7 +6780,7 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>35</v>
@@ -6888,7 +6855,7 @@
         <v>52</v>
       </c>
       <c r="Z54" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AA54" s="4" t="n">
         <v>1</v>
@@ -6914,7 +6881,7 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>35</v>
@@ -6950,7 +6917,7 @@
         <v>39</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>39</v>
@@ -6989,7 +6956,7 @@
         <v>52</v>
       </c>
       <c r="Z55" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AA55" s="4" t="n">
         <v>3</v>
@@ -7015,7 +6982,7 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>35</v>
@@ -7051,7 +7018,7 @@
         <v>39</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>39</v>
@@ -7090,7 +7057,7 @@
         <v>52</v>
       </c>
       <c r="Z56" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AA56" s="4" t="n">
         <v>1</v>
@@ -7116,7 +7083,7 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>35</v>
@@ -7191,7 +7158,7 @@
         <v>52</v>
       </c>
       <c r="Z57" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AA57" s="4" t="n">
         <v>1</v>
@@ -7217,7 +7184,7 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>35</v>
@@ -7250,7 +7217,7 @@
         <v>1</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>40</v>
@@ -7292,7 +7259,7 @@
         <v>52</v>
       </c>
       <c r="Z58" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA58" s="1" t="n">
         <v>1</v>
@@ -7318,7 +7285,7 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>35</v>
@@ -7351,7 +7318,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>40</v>
@@ -7419,7 +7386,7 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>35</v>
@@ -7452,10 +7419,10 @@
         <v>1</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>77</v>
@@ -7494,7 +7461,7 @@
         <v>52</v>
       </c>
       <c r="Z60" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AA60" s="1" t="n">
         <v>1</v>
@@ -7520,7 +7487,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>35</v>
@@ -7577,7 +7544,7 @@
         <v>86</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U61" s="1" t="s">
         <v>39</v>
@@ -7621,7 +7588,7 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>35</v>
@@ -7657,7 +7624,7 @@
         <v>80</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>77</v>
@@ -7678,7 +7645,7 @@
         <v>86</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U62" s="1" t="s">
         <v>39</v>
@@ -7722,7 +7689,7 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>35</v>
@@ -7779,7 +7746,7 @@
         <v>86</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U63" s="1" t="s">
         <v>39</v>
@@ -7803,7 +7770,7 @@
         <v>1</v>
       </c>
       <c r="AB63" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC63" s="8" t="s">
         <v>39</v>
@@ -7823,7 +7790,7 @@
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>35</v>
@@ -7850,7 +7817,7 @@
         <v>38</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K64" s="15" t="n">
         <v>1</v>
@@ -7898,7 +7865,7 @@
         <v>52</v>
       </c>
       <c r="Z64" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA64" s="1" t="n">
         <v>1</v>
@@ -7924,7 +7891,7 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>35</v>
@@ -7957,7 +7924,7 @@
         <v>39</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>40</v>
@@ -7999,7 +7966,7 @@
         <v>52</v>
       </c>
       <c r="Z65" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA65" s="1" t="n">
         <v>1</v>
@@ -8025,7 +7992,7 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>35</v>
@@ -8058,7 +8025,7 @@
         <v>39</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>40</v>
@@ -8091,7 +8058,7 @@
         <v>43</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X66" s="1" t="s">
         <v>44</v>
@@ -8100,7 +8067,7 @@
         <v>52</v>
       </c>
       <c r="Z66" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA66" s="1" t="n">
         <v>1</v>
@@ -8126,7 +8093,7 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>35</v>
@@ -8201,7 +8168,7 @@
         <v>52</v>
       </c>
       <c r="Z67" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA67" s="1" t="n">
         <v>1</v>
@@ -8227,7 +8194,7 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>35</v>
@@ -8308,7 +8275,7 @@
         <v>1</v>
       </c>
       <c r="AB68" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC68" s="8" t="s">
         <v>39</v>
@@ -8328,7 +8295,7 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>35</v>
@@ -8429,7 +8396,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>35</v>
@@ -8530,7 +8497,7 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>35</v>
@@ -8631,7 +8598,7 @@
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>35</v>
@@ -8732,7 +8699,7 @@
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>35</v>
@@ -8833,7 +8800,7 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>35</v>
@@ -8866,13 +8833,13 @@
         <v>1</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O74" s="10" t="n">
         <v>45384</v>
@@ -8934,7 +8901,7 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>35</v>
@@ -8967,13 +8934,13 @@
         <v>1</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O75" s="10" t="n">
         <v>45384</v>
@@ -8988,10 +8955,10 @@
         <v>7709577438</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T75" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U75" s="1" t="s">
         <v>39</v>
@@ -9035,7 +9002,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>35</v>
@@ -9068,13 +9035,13 @@
         <v>1</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="O76" s="10" t="n">
         <v>45384</v>
@@ -9089,10 +9056,10 @@
         <v>6060606060</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T76" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U76" s="1" t="s">
         <v>39</v>
@@ -9136,7 +9103,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>35</v>
@@ -9169,13 +9136,13 @@
         <v>1</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O77" s="10" t="n">
         <v>45384</v>
@@ -9190,10 +9157,10 @@
         <v>7070707070</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T77" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U77" s="1" t="s">
         <v>39</v>
@@ -9223,7 +9190,7 @@
         <v>39</v>
       </c>
       <c r="AD77" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE77" s="8" t="s">
         <v>39</v>
@@ -9237,7 +9204,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>35</v>
@@ -9270,13 +9237,13 @@
         <v>1</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O78" s="10" t="n">
         <v>45384</v>
@@ -9291,10 +9258,10 @@
         <v>7070707070</v>
       </c>
       <c r="S78" s="20" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="T78" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U78" s="1" t="s">
         <v>39</v>
@@ -9338,7 +9305,7 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>35</v>
@@ -9374,7 +9341,7 @@
         <v>80</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>77</v>
@@ -9395,7 +9362,7 @@
         <v>86</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U79" s="1" t="s">
         <v>39</v>
@@ -9419,13 +9386,13 @@
         <v>1</v>
       </c>
       <c r="AB79" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC79" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AD79" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AE79" s="8" t="s">
         <v>39</v>
@@ -9439,7 +9406,7 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>35</v>
@@ -9472,13 +9439,13 @@
         <v>1</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O80" s="10" t="n">
         <v>45384</v>
@@ -9520,7 +9487,7 @@
         <v>1</v>
       </c>
       <c r="AB80" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC80" s="8" t="s">
         <v>39</v>
@@ -9540,7 +9507,7 @@
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>35</v>
@@ -9573,13 +9540,13 @@
         <v>1</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O81" s="10" t="n">
         <v>45384</v>
@@ -9621,13 +9588,13 @@
         <v>1</v>
       </c>
       <c r="AB81" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC81" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AD81" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AE81" s="8" t="s">
         <v>39</v>
@@ -9640,108 +9607,108 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G82" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>600</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J82" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M82" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B82" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D82" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F82" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G82" s="21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H82" s="21" t="n">
-        <v>600</v>
-      </c>
-      <c r="I82" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J82" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="K82" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="L82" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="M82" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="N82" s="21" t="s">
+      <c r="N82" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O82" s="27" t="n">
+      <c r="O82" s="10" t="n">
         <v>45384</v>
       </c>
-      <c r="P82" s="27" t="s">
+      <c r="P82" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q82" s="27" t="s">
+      <c r="Q82" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="R82" s="28" t="n">
+      <c r="R82" s="11" t="n">
         <v>7709577438</v>
       </c>
-      <c r="S82" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T82" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U82" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V82" s="21" t="s">
+      <c r="S82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U82" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V82" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="W82" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="X82" s="21" t="s">
+      <c r="W82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X82" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Y82" s="21" t="s">
+      <c r="Y82" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Z82" s="21" t="n">
+      <c r="Z82" s="4" t="n">
         <v>7719921544</v>
       </c>
-      <c r="AA82" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB82" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC82" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD82" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE82" s="21"/>
-      <c r="AF82" s="21"/>
+      <c r="AA82" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB82" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC82" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE82" s="4"/>
+      <c r="AF82" s="4"/>
       <c r="AG82" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="83" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>36</v>
@@ -9762,7 +9729,7 @@
         <v>600</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J83" s="9" t="n">
         <v>1</v>
@@ -9795,7 +9762,7 @@
         <v>39</v>
       </c>
       <c r="T83" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U83" s="4" t="s">
         <v>39</v>
@@ -9831,15 +9798,15 @@
         <v>39</v>
       </c>
       <c r="AF83" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>36</v>
@@ -9860,7 +9827,7 @@
         <v>600</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J84" s="9" t="n">
         <v>1</v>
@@ -9869,10 +9836,10 @@
         <v>1</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>39</v>
@@ -9929,15 +9896,15 @@
         <v>39</v>
       </c>
       <c r="AF84" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>36</v>
@@ -9958,7 +9925,7 @@
         <v>600</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J85" s="9" t="n">
         <v>1</v>
@@ -9967,10 +9934,10 @@
         <v>1</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>39</v>
@@ -10027,15 +9994,15 @@
         <v>39</v>
       </c>
       <c r="AF85" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" s="4" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>36</v>
@@ -10056,7 +10023,7 @@
         <v>600</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J86" s="9" t="n">
         <v>1</v>
@@ -10065,10 +10032,10 @@
         <v>1</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>39</v>
@@ -10125,18 +10092,18 @@
         <v>39</v>
       </c>
       <c r="AF86" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG86" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>36</v>
@@ -10157,7 +10124,7 @@
         <v>600</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J87" s="9" t="n">
         <v>1</v>
@@ -10166,10 +10133,10 @@
         <v>1</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>39</v>
@@ -10226,15 +10193,15 @@
         <v>39</v>
       </c>
       <c r="AF87" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C88" s="13" t="s">
         <v>36</v>
@@ -10243,7 +10210,7 @@
         <v>123456</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F88" s="3" t="n">
         <v>123456</v>
@@ -10255,7 +10222,7 @@
         <v>600</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J88" s="9" t="n">
         <v>1</v>
@@ -10264,10 +10231,10 @@
         <v>1</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>39</v>
@@ -10328,419 +10295,403 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B89" s="22" t="s">
+      <c r="A89" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="23" t="s">
+      <c r="C89" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D89" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E89" s="21" t="s">
+      <c r="D89" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="J89" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="K89" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="L89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="M89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="N89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="P89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="R89" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="S89" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T89" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="W89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="X89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF89" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG89" s="0"/>
-      <c r="AH89" s="0"/>
-      <c r="AI89" s="0"/>
-      <c r="AJ89" s="0"/>
+      <c r="F89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="X89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE89" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF89" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="22" t="s">
+      <c r="A90" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C90" s="23" t="s">
+      <c r="C90" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D90" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E90" s="21" t="s">
+      <c r="D90" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F90" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G90" s="21" t="n">
+      <c r="F90" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G90" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="H90" s="21" t="n">
+      <c r="H90" s="4" t="n">
         <v>600</v>
       </c>
-      <c r="I90" s="24" t="s">
+      <c r="I90" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J90" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="K90" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="L90" s="24" t="s">
+      <c r="J90" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M90" s="24" t="s">
+      <c r="M90" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N90" s="21" t="s">
+      <c r="N90" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O90" s="27" t="n">
+      <c r="O90" s="10" t="n">
         <v>45384</v>
       </c>
-      <c r="P90" s="27" t="s">
+      <c r="P90" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q90" s="27" t="s">
+      <c r="Q90" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="R90" s="28" t="n">
+      <c r="R90" s="11" t="n">
         <v>7350513300</v>
       </c>
-      <c r="S90" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T90" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U90" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V90" s="21" t="s">
+      <c r="S90" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T90" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U90" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V90" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="W90" s="24" t="s">
+      <c r="W90" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="X90" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y90" s="21" t="s">
+      <c r="X90" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y90" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Z90" s="28" t="n">
+      <c r="Z90" s="11" t="n">
         <v>7350513300</v>
       </c>
-      <c r="AA90" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB90" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC90" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD90" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE90" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF90" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG90" s="0"/>
-      <c r="AH90" s="0"/>
-      <c r="AI90" s="0"/>
-      <c r="AJ90" s="0"/>
+      <c r="AA90" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB90" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC90" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD90" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE90" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF90" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="B91" s="22" t="s">
+      <c r="A91" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C91" s="22" t="s">
+      <c r="C91" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D91" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E91" s="21" t="s">
+      <c r="D91" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G91" s="21" t="n">
+      <c r="F91" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G91" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="H91" s="21" t="n">
+      <c r="H91" s="4" t="n">
         <v>600</v>
       </c>
-      <c r="I91" s="24" t="s">
+      <c r="I91" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J91" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="K91" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="L91" s="24" t="s">
+      <c r="J91" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L91" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M91" s="24" t="s">
+      <c r="M91" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N91" s="21" t="s">
+      <c r="N91" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O91" s="27" t="n">
+      <c r="O91" s="10" t="n">
         <v>45384</v>
       </c>
-      <c r="P91" s="27" t="s">
+      <c r="P91" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q91" s="27" t="s">
+      <c r="Q91" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="R91" s="28" t="n">
+      <c r="R91" s="11" t="n">
         <v>7350516600</v>
       </c>
-      <c r="S91" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T91" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U91" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V91" s="21" t="s">
+      <c r="S91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U91" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V91" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="W91" s="24" t="s">
+      <c r="W91" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="X91" s="21" t="s">
+      <c r="X91" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Y91" s="21" t="s">
+      <c r="Y91" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Z91" s="28" t="n">
+      <c r="Z91" s="11" t="n">
         <v>7350516600</v>
       </c>
-      <c r="AA91" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB91" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC91" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD91" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE91" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF91" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG91" s="0"/>
-      <c r="AH91" s="0"/>
-      <c r="AI91" s="0"/>
-      <c r="AJ91" s="0"/>
+      <c r="AA91" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB91" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC91" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE91" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF91" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="B92" s="22" t="s">
+      <c r="A92" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C92" s="22" t="s">
+      <c r="C92" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D92" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E92" s="21" t="s">
+      <c r="D92" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F92" s="22" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G92" s="21" t="n">
+      <c r="F92" s="3" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G92" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="H92" s="21" t="n">
+      <c r="H92" s="4" t="n">
         <v>600</v>
       </c>
-      <c r="I92" s="24" t="s">
+      <c r="I92" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J92" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="K92" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="L92" s="24" t="s">
+      <c r="J92" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K92" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L92" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M92" s="24" t="s">
+      <c r="M92" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N92" s="21" t="s">
+      <c r="N92" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O92" s="27" t="n">
+      <c r="O92" s="10" t="n">
         <v>45384</v>
       </c>
-      <c r="P92" s="27" t="s">
+      <c r="P92" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q92" s="27" t="s">
+      <c r="Q92" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="R92" s="28" t="n">
+      <c r="R92" s="11" t="n">
         <v>9911882277</v>
       </c>
-      <c r="S92" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="T92" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="U92" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="V92" s="21" t="s">
+      <c r="S92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U92" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V92" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="W92" s="24" t="s">
+      <c r="W92" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="X92" s="21" t="s">
+      <c r="X92" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Y92" s="21" t="s">
+      <c r="Y92" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="Z92" s="28" t="n">
+      <c r="Z92" s="11" t="n">
         <v>9911882277</v>
       </c>
-      <c r="AA92" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB92" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC92" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD92" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE92" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF92" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG92" s="0"/>
-      <c r="AH92" s="0"/>
-      <c r="AI92" s="0"/>
-      <c r="AJ92" s="0"/>
+      <c r="AA92" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB92" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC92" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE92" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF92" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>36</v>
@@ -10763,19 +10714,19 @@
       <c r="I93" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J93" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K93" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L93" s="30" t="s">
+      <c r="J93" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K93" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L93" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M93" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N93" s="30" t="s">
+      <c r="N93" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O93" s="6" t="n">
@@ -10838,10 +10789,10 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>36</v>
@@ -10864,19 +10815,19 @@
       <c r="I94" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J94" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K94" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L94" s="30" t="s">
+      <c r="J94" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K94" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L94" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M94" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N94" s="30" t="s">
+      <c r="N94" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O94" s="6" t="n">
@@ -10939,10 +10890,10 @@
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>36</v>
@@ -10965,19 +10916,19 @@
       <c r="I95" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J95" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K95" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L95" s="30" t="s">
+      <c r="J95" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K95" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L95" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M95" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N95" s="30" t="s">
+      <c r="N95" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O95" s="6" t="n">
@@ -11040,10 +10991,10 @@
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>36</v>
@@ -11052,7 +11003,7 @@
         <v>123456</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F96" s="3" t="n">
         <v>123456</v>
@@ -11066,19 +11017,19 @@
       <c r="I96" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J96" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K96" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L96" s="30" t="s">
+      <c r="J96" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K96" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L96" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M96" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N96" s="30" t="s">
+      <c r="N96" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O96" s="6" t="n">
@@ -11141,10 +11092,10 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>36</v>
@@ -11167,19 +11118,19 @@
       <c r="I97" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J97" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K97" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L97" s="30" t="s">
+      <c r="J97" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K97" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L97" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M97" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N97" s="30" t="s">
+      <c r="N97" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O97" s="6" t="n">
@@ -11216,7 +11167,7 @@
         <v>52</v>
       </c>
       <c r="Z97" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA97" s="5" t="s">
         <v>39</v>
@@ -11242,10 +11193,10 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>36</v>
@@ -11268,19 +11219,19 @@
       <c r="I98" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J98" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K98" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L98" s="30" t="s">
+      <c r="J98" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K98" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L98" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M98" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N98" s="30" t="s">
+      <c r="N98" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O98" s="6" t="n">
@@ -11343,10 +11294,10 @@
     </row>
     <row r="99" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>36</v>
@@ -11369,19 +11320,19 @@
       <c r="I99" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J99" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K99" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L99" s="30" t="s">
+      <c r="J99" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K99" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L99" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M99" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N99" s="30" t="s">
+      <c r="N99" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O99" s="6" t="n">
@@ -11441,10 +11392,10 @@
     </row>
     <row r="100" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>36</v>
@@ -11467,19 +11418,19 @@
       <c r="I100" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J100" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K100" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L100" s="30" t="s">
+      <c r="J100" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K100" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L100" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M100" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N100" s="30" t="s">
+      <c r="N100" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O100" s="6" t="n">
@@ -11516,7 +11467,7 @@
         <v>52</v>
       </c>
       <c r="Z100" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AA100" s="5" t="s">
         <v>39</v>
@@ -11542,10 +11493,10 @@
     </row>
     <row r="101" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>36</v>
@@ -11568,19 +11519,19 @@
       <c r="I101" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J101" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K101" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L101" s="30" t="s">
+      <c r="J101" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K101" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L101" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M101" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N101" s="30" t="s">
+      <c r="N101" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O101" s="6" t="n">
@@ -11617,7 +11568,7 @@
         <v>55</v>
       </c>
       <c r="Z101" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AA101" s="5" t="s">
         <v>39</v>
@@ -11643,10 +11594,10 @@
     </row>
     <row r="102" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>36</v>
@@ -11669,19 +11620,19 @@
       <c r="I102" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J102" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K102" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L102" s="30" t="s">
+      <c r="J102" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K102" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L102" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M102" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N102" s="30" t="s">
+      <c r="N102" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O102" s="6" t="n">
@@ -11744,10 +11695,10 @@
     </row>
     <row r="103" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>36</v>
@@ -11770,19 +11721,19 @@
       <c r="I103" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J103" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K103" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L103" s="30" t="s">
+      <c r="J103" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K103" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L103" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M103" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N103" s="30" t="s">
+      <c r="N103" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O103" s="6" t="n">
@@ -11845,10 +11796,10 @@
     </row>
     <row r="104" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>36</v>
@@ -11871,19 +11822,19 @@
       <c r="I104" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J104" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K104" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L104" s="30" t="s">
+      <c r="J104" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K104" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L104" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M104" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N104" s="30" t="s">
+      <c r="N104" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O104" s="6" t="n">
@@ -11920,7 +11871,7 @@
         <v>59</v>
       </c>
       <c r="Z104" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA104" s="5" t="s">
         <v>39</v>
@@ -11946,10 +11897,10 @@
     </row>
     <row r="105" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>36</v>
@@ -11972,19 +11923,19 @@
       <c r="I105" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J105" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K105" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L105" s="30" t="s">
+      <c r="J105" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K105" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L105" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M105" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N105" s="30" t="s">
+      <c r="N105" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O105" s="6" t="n">
@@ -12021,7 +11972,7 @@
         <v>55</v>
       </c>
       <c r="Z105" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA105" s="5" t="s">
         <v>39</v>
@@ -12047,10 +11998,10 @@
     </row>
     <row r="106" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>36</v>
@@ -12073,19 +12024,19 @@
       <c r="I106" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J106" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K106" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L106" s="30" t="s">
+      <c r="J106" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K106" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L106" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M106" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N106" s="30" t="s">
+      <c r="N106" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O106" s="6" t="n">
@@ -12122,7 +12073,7 @@
         <v>52</v>
       </c>
       <c r="Z106" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AA106" s="5" t="s">
         <v>39</v>
@@ -12148,10 +12099,10 @@
     </row>
     <row r="107" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>36</v>
@@ -12174,19 +12125,19 @@
       <c r="I107" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J107" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K107" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L107" s="30" t="s">
+      <c r="J107" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K107" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L107" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M107" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N107" s="30" t="s">
+      <c r="N107" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O107" s="6" t="n">
@@ -12223,7 +12174,7 @@
         <v>52</v>
       </c>
       <c r="Z107" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AA107" s="5" t="s">
         <v>39</v>
@@ -12249,10 +12200,10 @@
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>36</v>
@@ -12275,19 +12226,19 @@
       <c r="I108" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J108" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K108" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L108" s="30" t="s">
+      <c r="J108" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K108" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L108" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M108" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N108" s="30" t="s">
+      <c r="N108" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O108" s="6" t="n">
@@ -12324,7 +12275,7 @@
         <v>52</v>
       </c>
       <c r="Z108" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA108" s="1" t="n">
         <v>1</v>
@@ -12350,10 +12301,10 @@
     </row>
     <row r="109" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>36</v>
@@ -12376,19 +12327,19 @@
       <c r="I109" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J109" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K109" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L109" s="30" t="s">
+      <c r="J109" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K109" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L109" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M109" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N109" s="30" t="s">
+      <c r="N109" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O109" s="6" t="n">
@@ -12451,10 +12402,10 @@
     </row>
     <row r="110" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>36</v>
@@ -12477,19 +12428,19 @@
       <c r="I110" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J110" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K110" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L110" s="30" t="s">
+      <c r="J110" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K110" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L110" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M110" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N110" s="30" t="s">
+      <c r="N110" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O110" s="6" t="n">
@@ -12552,10 +12503,10 @@
     </row>
     <row r="111" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>36</v>
@@ -12578,19 +12529,19 @@
       <c r="I111" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J111" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K111" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L111" s="30" t="s">
+      <c r="J111" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K111" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L111" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M111" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N111" s="30" t="s">
+      <c r="N111" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O111" s="6" t="n">
@@ -12653,10 +12604,10 @@
     </row>
     <row r="112" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>36</v>
@@ -12679,19 +12630,19 @@
       <c r="I112" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J112" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K112" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L112" s="30" t="s">
+      <c r="J112" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K112" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L112" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M112" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N112" s="30" t="s">
+      <c r="N112" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O112" s="6" t="n">
@@ -12754,10 +12705,10 @@
     </row>
     <row r="113" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>36</v>
@@ -12780,19 +12731,19 @@
       <c r="I113" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J113" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K113" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L113" s="30" t="s">
+      <c r="J113" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K113" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L113" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M113" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N113" s="30" t="s">
+      <c r="N113" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O113" s="6" t="n">
@@ -12829,7 +12780,7 @@
         <v>52</v>
       </c>
       <c r="Z113" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA113" s="5" t="s">
         <v>39</v>
@@ -12855,10 +12806,10 @@
     </row>
     <row r="114" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>36</v>
@@ -12881,19 +12832,19 @@
       <c r="I114" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J114" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K114" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L114" s="30" t="s">
+      <c r="J114" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K114" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L114" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M114" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N114" s="30" t="s">
+      <c r="N114" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O114" s="6" t="n">
@@ -12930,7 +12881,7 @@
         <v>52</v>
       </c>
       <c r="Z114" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA114" s="5" t="s">
         <v>39</v>
@@ -12956,10 +12907,10 @@
     </row>
     <row r="115" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>36</v>
@@ -12982,19 +12933,19 @@
       <c r="I115" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J115" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K115" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L115" s="30" t="s">
+      <c r="J115" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K115" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L115" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M115" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N115" s="30" t="s">
+      <c r="N115" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O115" s="6" t="n">
@@ -13031,7 +12982,7 @@
         <v>52</v>
       </c>
       <c r="Z115" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA115" s="1" t="n">
         <v>0</v>
@@ -13057,10 +13008,10 @@
     </row>
     <row r="116" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>36</v>
@@ -13083,19 +13034,19 @@
       <c r="I116" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J116" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K116" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L116" s="30" t="s">
+      <c r="J116" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K116" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L116" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M116" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N116" s="30" t="s">
+      <c r="N116" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O116" s="6" t="n">
@@ -13132,7 +13083,7 @@
         <v>52</v>
       </c>
       <c r="Z116" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA116" s="1" t="n">
         <v>1</v>
@@ -13158,10 +13109,10 @@
     </row>
     <row r="117" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>36</v>
@@ -13184,19 +13135,19 @@
       <c r="I117" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J117" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K117" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L117" s="30" t="s">
+      <c r="J117" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K117" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L117" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M117" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N117" s="30" t="s">
+      <c r="N117" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O117" s="6" t="n">
@@ -13233,7 +13184,7 @@
         <v>52</v>
       </c>
       <c r="Z117" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA117" s="1" t="n">
         <v>1</v>
@@ -13259,10 +13210,10 @@
     </row>
     <row r="118" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>36</v>
@@ -13285,19 +13236,19 @@
       <c r="I118" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J118" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K118" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L118" s="30" t="s">
+      <c r="J118" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K118" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L118" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M118" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N118" s="30" t="s">
+      <c r="N118" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O118" s="6" t="n">
@@ -13334,7 +13285,7 @@
         <v>52</v>
       </c>
       <c r="Z118" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA118" s="1" t="n">
         <v>1</v>
@@ -13360,10 +13311,10 @@
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>36</v>
@@ -13372,7 +13323,7 @@
         <v>123456</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F119" s="3" t="n">
         <v>123456</v>
@@ -13386,19 +13337,19 @@
       <c r="I119" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J119" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K119" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L119" s="30" t="s">
+      <c r="J119" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K119" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L119" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M119" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N119" s="30" t="s">
+      <c r="N119" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O119" s="6" t="n">
@@ -13435,7 +13386,7 @@
         <v>52</v>
       </c>
       <c r="Z119" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA119" s="1" t="n">
         <v>1</v>
@@ -13461,10 +13412,10 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>36</v>
@@ -13487,19 +13438,19 @@
       <c r="I120" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J120" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K120" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L120" s="30" t="s">
+      <c r="J120" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K120" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L120" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M120" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N120" s="30" t="s">
+      <c r="N120" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O120" s="6" t="n">
@@ -13536,7 +13487,7 @@
         <v>52</v>
       </c>
       <c r="Z120" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA120" s="1" t="n">
         <v>1</v>
@@ -13562,10 +13513,10 @@
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>36</v>
@@ -13588,19 +13539,19 @@
       <c r="I121" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J121" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K121" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L121" s="30" t="s">
+      <c r="J121" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K121" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L121" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M121" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N121" s="30" t="s">
+      <c r="N121" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O121" s="6" t="n">
@@ -13637,7 +13588,7 @@
         <v>52</v>
       </c>
       <c r="Z121" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA121" s="1" t="n">
         <v>1</v>
@@ -13663,10 +13614,10 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>36</v>
@@ -13689,19 +13640,19 @@
       <c r="I122" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J122" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K122" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L122" s="30" t="s">
+      <c r="J122" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K122" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L122" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M122" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N122" s="30" t="s">
+      <c r="N122" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O122" s="6" t="n">
@@ -13738,7 +13689,7 @@
         <v>52</v>
       </c>
       <c r="Z122" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA122" s="1" t="n">
         <v>1</v>
@@ -13764,10 +13715,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>36</v>
@@ -13790,19 +13741,19 @@
       <c r="I123" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J123" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K123" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L123" s="30" t="s">
+      <c r="J123" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K123" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L123" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M123" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N123" s="30" t="s">
+      <c r="N123" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O123" s="6" t="n">
@@ -13839,7 +13790,7 @@
         <v>52</v>
       </c>
       <c r="Z123" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA123" s="1" t="n">
         <v>1</v>
@@ -13865,10 +13816,10 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>36</v>
@@ -13891,19 +13842,19 @@
       <c r="I124" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J124" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K124" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L124" s="30" t="s">
+      <c r="J124" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K124" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L124" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M124" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N124" s="30" t="s">
+      <c r="N124" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O124" s="6" t="n">
@@ -13940,7 +13891,7 @@
         <v>52</v>
       </c>
       <c r="Z124" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA124" s="1" t="n">
         <v>1</v>
@@ -13955,7 +13906,7 @@
         <v>39</v>
       </c>
       <c r="AE124" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AF124" s="8" t="s">
         <v>39</v>
@@ -13966,10 +13917,10 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>36</v>
@@ -13992,19 +13943,19 @@
       <c r="I125" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J125" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K125" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L125" s="30" t="s">
+      <c r="J125" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K125" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L125" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M125" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N125" s="30" t="s">
+      <c r="N125" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O125" s="6" t="n">
@@ -14041,7 +13992,7 @@
         <v>52</v>
       </c>
       <c r="Z125" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA125" s="1" t="n">
         <v>1</v>
@@ -14056,7 +14007,7 @@
         <v>39</v>
       </c>
       <c r="AE125" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AF125" s="8" t="s">
         <v>39</v>
@@ -14067,10 +14018,10 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>36</v>
@@ -14093,19 +14044,19 @@
       <c r="I126" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J126" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K126" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L126" s="30" t="s">
+      <c r="J126" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K126" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L126" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M126" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N126" s="30" t="s">
+      <c r="N126" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O126" s="6" t="n">
@@ -14142,7 +14093,7 @@
         <v>52</v>
       </c>
       <c r="Z126" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA126" s="1" t="n">
         <v>1</v>
@@ -14157,7 +14108,7 @@
         <v>39</v>
       </c>
       <c r="AE126" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AF126" s="8" t="s">
         <v>39</v>
@@ -14168,10 +14119,10 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>36</v>
@@ -14194,19 +14145,19 @@
       <c r="I127" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J127" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K127" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L127" s="30" t="s">
+      <c r="J127" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K127" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L127" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M127" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N127" s="30" t="s">
+      <c r="N127" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O127" s="6" t="n">
@@ -14243,7 +14194,7 @@
         <v>52</v>
       </c>
       <c r="Z127" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA127" s="1" t="n">
         <v>1</v>
@@ -14258,7 +14209,7 @@
         <v>39</v>
       </c>
       <c r="AE127" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AF127" s="8" t="s">
         <v>39</v>
@@ -14269,10 +14220,10 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>36</v>
@@ -14295,19 +14246,19 @@
       <c r="I128" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J128" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K128" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L128" s="30" t="s">
+      <c r="J128" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K128" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L128" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M128" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N128" s="30" t="s">
+      <c r="N128" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O128" s="6" t="n">
@@ -14344,7 +14295,7 @@
         <v>52</v>
       </c>
       <c r="Z128" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA128" s="1" t="n">
         <v>1</v>
@@ -14359,7 +14310,7 @@
         <v>39</v>
       </c>
       <c r="AE128" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AF128" s="8" t="s">
         <v>39</v>
@@ -14370,10 +14321,10 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>36</v>
@@ -14396,19 +14347,19 @@
       <c r="I129" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J129" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K129" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L129" s="30" t="s">
+      <c r="J129" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K129" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L129" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M129" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N129" s="30" t="s">
+      <c r="N129" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O129" s="6" t="n">
@@ -14445,7 +14396,7 @@
         <v>52</v>
       </c>
       <c r="Z129" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA129" s="1" t="n">
         <v>1</v>
@@ -14460,7 +14411,7 @@
         <v>39</v>
       </c>
       <c r="AE129" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AF129" s="8" t="s">
         <v>39</v>
@@ -14471,10 +14422,10 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>36</v>
@@ -14497,19 +14448,19 @@
       <c r="I130" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J130" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K130" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L130" s="30" t="s">
+      <c r="J130" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K130" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L130" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M130" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N130" s="30" t="s">
+      <c r="N130" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O130" s="6" t="n">
@@ -14546,7 +14497,7 @@
         <v>52</v>
       </c>
       <c r="Z130" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA130" s="1" t="n">
         <v>1</v>
@@ -14561,7 +14512,7 @@
         <v>39</v>
       </c>
       <c r="AE130" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AF130" s="8" t="s">
         <v>39</v>
@@ -14572,10 +14523,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>36</v>
@@ -14598,19 +14549,19 @@
       <c r="I131" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J131" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K131" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L131" s="30" t="s">
+      <c r="J131" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K131" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L131" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M131" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N131" s="30" t="s">
+      <c r="N131" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O131" s="6" t="n">
@@ -14647,7 +14598,7 @@
         <v>52</v>
       </c>
       <c r="Z131" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA131" s="1" t="n">
         <v>1</v>
@@ -14662,7 +14613,7 @@
         <v>39</v>
       </c>
       <c r="AE131" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AF131" s="8" t="s">
         <v>39</v>
@@ -14673,10 +14624,10 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>36</v>
@@ -14699,19 +14650,19 @@
       <c r="I132" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J132" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K132" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L132" s="30" t="s">
+      <c r="J132" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K132" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L132" s="21" t="s">
         <v>39</v>
       </c>
       <c r="M132" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N132" s="30" t="s">
+      <c r="N132" s="21" t="s">
         <v>39</v>
       </c>
       <c r="O132" s="6" t="n">
@@ -14748,7 +14699,7 @@
         <v>52</v>
       </c>
       <c r="Z132" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA132" s="1" t="n">
         <v>1</v>
@@ -14760,7 +14711,7 @@
         <v>39</v>
       </c>
       <c r="AE132" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AF132" s="8" t="s">
         <v>39</v>
@@ -14771,82 +14722,82 @@
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applying Tags After Module Run
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Exchange/exchange_test_data.xlsx
+++ b/TestData/Web_POS/Exchange/exchange_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="292">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -247,22 +247,28 @@
     <t xml:space="preserve">E_20</t>
   </si>
   <si>
+    <t xml:space="preserve">8906118412556 : 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">E_21</t>
   </si>
   <si>
     <t xml:space="preserve">cash : 275 , paytm : 275</t>
   </si>
   <si>
+    <t xml:space="preserve">8906118412662 : 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O5eza0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash : 100, paytm : 100, voucher : 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">8906118410781: 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O5eza0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cash : 100, paytm : 100, voucher : 0</t>
   </si>
   <si>
     <t xml:space="preserve">E_23</t>
@@ -1409,8 +1415,8 @@
   </sheetPr>
   <dimension ref="A1:AH148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S20" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA47" activeCellId="0" sqref="AA47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3482,8 +3488,8 @@
       <c r="L21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M21" s="5" t="s">
-        <v>40</v>
+      <c r="M21" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>39</v>
@@ -3539,13 +3545,13 @@
       <c r="AF21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AG21" s="8" t="s">
-        <v>39</v>
+      <c r="AG21" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>35</v>
@@ -3578,13 +3584,13 @@
         <v>1</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="O22" s="10" t="n">
         <v>45384</v>
@@ -3611,13 +3617,13 @@
         <v>43</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Z22" s="1" t="n">
         <v>7719921544</v>
@@ -3640,13 +3646,13 @@
       <c r="AF22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AG22" s="8" t="s">
-        <v>39</v>
+      <c r="AG22" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -3679,13 +3685,13 @@
         <v>1</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O23" s="10" t="n">
         <v>45384</v>
@@ -3712,7 +3718,7 @@
         <v>43</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X23" s="1" t="s">
         <v>44</v>
@@ -3747,7 +3753,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>35</v>
@@ -3780,13 +3786,13 @@
         <v>1</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O24" s="10" t="n">
         <v>45384</v>
@@ -3848,7 +3854,7 @@
     </row>
     <row r="25" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>35</v>
@@ -3881,13 +3887,13 @@
         <v>1</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O25" s="10" t="n">
         <v>45384</v>
@@ -3949,7 +3955,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>35</v>
@@ -3982,13 +3988,13 @@
         <v>1</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O26" s="10" t="n">
         <v>45384</v>
@@ -4050,7 +4056,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
@@ -4083,13 +4089,13 @@
         <v>1</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O27" s="10" t="n">
         <v>45384</v>
@@ -4151,7 +4157,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>35</v>
@@ -4184,13 +4190,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O28" s="10" t="n">
         <v>45384</v>
@@ -4205,7 +4211,7 @@
         <v>7709577438</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T28" s="2" t="s">
         <v>39</v>
@@ -4252,7 +4258,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>35</v>
@@ -4285,13 +4291,13 @@
         <v>1</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O29" s="10" t="n">
         <v>45384</v>
@@ -4318,7 +4324,7 @@
         <v>43</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X29" s="1" t="s">
         <v>44</v>
@@ -4353,7 +4359,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>35</v>
@@ -4386,13 +4392,13 @@
         <v>1</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O30" s="10" t="n">
         <v>45384</v>
@@ -4419,7 +4425,7 @@
         <v>43</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X30" s="1" t="s">
         <v>44</v>
@@ -4454,7 +4460,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>35</v>
@@ -4487,13 +4493,13 @@
         <v>1</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O31" s="10" t="n">
         <v>45384</v>
@@ -4555,7 +4561,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>35</v>
@@ -4588,13 +4594,13 @@
         <v>1</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O32" s="10" t="n">
         <v>45384</v>
@@ -4656,7 +4662,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
@@ -4689,13 +4695,13 @@
         <v>1</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O33" s="10" t="n">
         <v>45384</v>
@@ -4757,7 +4763,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>35</v>
@@ -4790,13 +4796,13 @@
         <v>1</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O34" s="10" t="n">
         <v>45384</v>
@@ -4858,7 +4864,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>35</v>
@@ -4891,13 +4897,13 @@
         <v>1</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O35" s="10" t="n">
         <v>45384</v>
@@ -4924,7 +4930,7 @@
         <v>43</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>44</v>
@@ -4959,7 +4965,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>35</v>
@@ -4992,13 +4998,13 @@
         <v>1</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O36" s="10" t="n">
         <v>45384</v>
@@ -5025,7 +5031,7 @@
         <v>43</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X36" s="1" t="s">
         <v>44</v>
@@ -5060,7 +5066,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>35</v>
@@ -5093,13 +5099,13 @@
         <v>1</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O37" s="10" t="n">
         <v>45384</v>
@@ -5161,7 +5167,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>35</v>
@@ -5194,13 +5200,13 @@
         <v>1</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O38" s="10" t="n">
         <v>45384</v>
@@ -5262,7 +5268,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>35</v>
@@ -5295,13 +5301,13 @@
         <v>1</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O39" s="10" t="n">
         <v>45384</v>
@@ -5363,7 +5369,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>35</v>
@@ -5396,13 +5402,13 @@
         <v>1</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O40" s="10" t="n">
         <v>45384</v>
@@ -5464,7 +5470,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>35</v>
@@ -5497,13 +5503,13 @@
         <v>1</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O41" s="10" t="n">
         <v>45384</v>
@@ -5530,7 +5536,7 @@
         <v>43</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X41" s="1" t="s">
         <v>44</v>
@@ -5565,7 +5571,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>35</v>
@@ -5601,7 +5607,7 @@
         <v>39</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>39</v>
@@ -5640,7 +5646,7 @@
         <v>52</v>
       </c>
       <c r="Z42" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AA42" s="4" t="n">
         <v>1</v>
@@ -5666,7 +5672,7 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>35</v>
@@ -5702,7 +5708,7 @@
         <v>39</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>39</v>
@@ -5741,7 +5747,7 @@
         <v>52</v>
       </c>
       <c r="Z43" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AA43" s="4" t="n">
         <v>1</v>
@@ -5767,7 +5773,7 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>35</v>
@@ -5803,7 +5809,7 @@
         <v>39</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>39</v>
@@ -5842,7 +5848,7 @@
         <v>52</v>
       </c>
       <c r="Z44" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AA44" s="4" t="n">
         <v>1</v>
@@ -5868,7 +5874,7 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>35</v>
@@ -5904,7 +5910,7 @@
         <v>39</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>39</v>
@@ -5943,7 +5949,7 @@
         <v>52</v>
       </c>
       <c r="Z45" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AA45" s="4" t="n">
         <v>1</v>
@@ -5972,7 +5978,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>35</v>
@@ -6008,7 +6014,7 @@
         <v>39</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>39</v>
@@ -6047,7 +6053,7 @@
         <v>52</v>
       </c>
       <c r="Z46" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AA46" s="4" t="n">
         <v>2</v>
@@ -6073,7 +6079,7 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>35</v>
@@ -6109,7 +6115,7 @@
         <v>39</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>39</v>
@@ -6148,7 +6154,7 @@
         <v>52</v>
       </c>
       <c r="Z47" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AA47" s="4" t="n">
         <v>3</v>
@@ -6174,7 +6180,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>35</v>
@@ -6210,7 +6216,7 @@
         <v>39</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>39</v>
@@ -6249,7 +6255,7 @@
         <v>52</v>
       </c>
       <c r="Z48" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AA48" s="4" t="n">
         <v>4</v>
@@ -6275,7 +6281,7 @@
     </row>
     <row r="49" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>35</v>
@@ -6302,7 +6308,7 @@
         <v>38</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K49" s="15" t="n">
         <v>1</v>
@@ -6350,7 +6356,7 @@
         <v>52</v>
       </c>
       <c r="Z49" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AA49" s="4" t="n">
         <v>1</v>
@@ -6376,7 +6382,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>35</v>
@@ -6412,7 +6418,7 @@
         <v>39</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>39</v>
@@ -6451,7 +6457,7 @@
         <v>52</v>
       </c>
       <c r="Z50" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AA50" s="4" t="n">
         <v>1</v>
@@ -6477,7 +6483,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>35</v>
@@ -6552,7 +6558,7 @@
         <v>52</v>
       </c>
       <c r="Z51" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AA51" s="4" t="n">
         <v>1</v>
@@ -6578,7 +6584,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>35</v>
@@ -6653,7 +6659,7 @@
         <v>52</v>
       </c>
       <c r="Z52" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AA52" s="4" t="n">
         <v>1</v>
@@ -6679,7 +6685,7 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>35</v>
@@ -6754,7 +6760,7 @@
         <v>52</v>
       </c>
       <c r="Z53" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AA53" s="4" t="n">
         <v>3</v>
@@ -6780,7 +6786,7 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>35</v>
@@ -6855,7 +6861,7 @@
         <v>52</v>
       </c>
       <c r="Z54" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AA54" s="4" t="n">
         <v>1</v>
@@ -6881,7 +6887,7 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>35</v>
@@ -6917,7 +6923,7 @@
         <v>39</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>39</v>
@@ -6956,7 +6962,7 @@
         <v>52</v>
       </c>
       <c r="Z55" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AA55" s="4" t="n">
         <v>3</v>
@@ -6982,7 +6988,7 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>35</v>
@@ -7018,7 +7024,7 @@
         <v>39</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>39</v>
@@ -7057,7 +7063,7 @@
         <v>52</v>
       </c>
       <c r="Z56" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AA56" s="4" t="n">
         <v>1</v>
@@ -7083,7 +7089,7 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>35</v>
@@ -7158,7 +7164,7 @@
         <v>52</v>
       </c>
       <c r="Z57" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AA57" s="4" t="n">
         <v>1</v>
@@ -7184,7 +7190,7 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>35</v>
@@ -7217,13 +7223,13 @@
         <v>1</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O58" s="10" t="n">
         <v>45384</v>
@@ -7259,7 +7265,7 @@
         <v>52</v>
       </c>
       <c r="Z58" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AA58" s="1" t="n">
         <v>1</v>
@@ -7285,7 +7291,7 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>35</v>
@@ -7318,13 +7324,13 @@
         <v>1</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O59" s="10" t="n">
         <v>45384</v>
@@ -7386,7 +7392,7 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>35</v>
@@ -7419,13 +7425,13 @@
         <v>1</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O60" s="10" t="n">
         <v>45384</v>
@@ -7461,7 +7467,7 @@
         <v>52</v>
       </c>
       <c r="Z60" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AA60" s="1" t="n">
         <v>1</v>
@@ -7487,7 +7493,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>35</v>
@@ -7520,13 +7526,13 @@
         <v>1</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O61" s="10" t="n">
         <v>45384</v>
@@ -7541,10 +7547,10 @@
         <v>7709577438</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U61" s="1" t="s">
         <v>39</v>
@@ -7588,7 +7594,7 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>35</v>
@@ -7621,13 +7627,13 @@
         <v>1</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O62" s="10" t="n">
         <v>45384</v>
@@ -7642,10 +7648,10 @@
         <v>7709577438</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U62" s="1" t="s">
         <v>39</v>
@@ -7689,7 +7695,7 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>35</v>
@@ -7722,13 +7728,13 @@
         <v>1</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M63" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O63" s="19" t="n">
         <v>45384</v>
@@ -7743,10 +7749,10 @@
         <v>7709577438</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U63" s="1" t="s">
         <v>39</v>
@@ -7770,7 +7776,7 @@
         <v>1</v>
       </c>
       <c r="AB63" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AC63" s="8" t="s">
         <v>39</v>
@@ -7790,7 +7796,7 @@
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>35</v>
@@ -7817,7 +7823,7 @@
         <v>38</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K64" s="15" t="n">
         <v>1</v>
@@ -7856,7 +7862,7 @@
         <v>43</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X64" s="1" t="s">
         <v>44</v>
@@ -7865,7 +7871,7 @@
         <v>52</v>
       </c>
       <c r="Z64" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AA64" s="1" t="n">
         <v>1</v>
@@ -7891,7 +7897,7 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>35</v>
@@ -7924,7 +7930,7 @@
         <v>39</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>40</v>
@@ -7957,7 +7963,7 @@
         <v>43</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X65" s="1" t="s">
         <v>44</v>
@@ -7966,7 +7972,7 @@
         <v>52</v>
       </c>
       <c r="Z65" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AA65" s="1" t="n">
         <v>1</v>
@@ -7992,7 +7998,7 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>35</v>
@@ -8025,7 +8031,7 @@
         <v>39</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>40</v>
@@ -8058,7 +8064,7 @@
         <v>43</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="X66" s="1" t="s">
         <v>44</v>
@@ -8067,7 +8073,7 @@
         <v>52</v>
       </c>
       <c r="Z66" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AA66" s="1" t="n">
         <v>1</v>
@@ -8093,7 +8099,7 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>35</v>
@@ -8126,13 +8132,13 @@
         <v>1</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M67" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O67" s="10" t="n">
         <v>45384</v>
@@ -8159,7 +8165,7 @@
         <v>43</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X67" s="1" t="s">
         <v>44</v>
@@ -8168,7 +8174,7 @@
         <v>52</v>
       </c>
       <c r="Z67" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AA67" s="1" t="n">
         <v>1</v>
@@ -8194,7 +8200,7 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>35</v>
@@ -8227,13 +8233,13 @@
         <v>1</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O68" s="10" t="n">
         <v>45384</v>
@@ -8260,7 +8266,7 @@
         <v>43</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X68" s="1" t="s">
         <v>44</v>
@@ -8275,7 +8281,7 @@
         <v>1</v>
       </c>
       <c r="AB68" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AC68" s="8" t="s">
         <v>39</v>
@@ -8295,7 +8301,7 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>35</v>
@@ -8328,13 +8334,13 @@
         <v>1</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M69" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O69" s="10" t="n">
         <v>45384</v>
@@ -8396,7 +8402,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>35</v>
@@ -8429,13 +8435,13 @@
         <v>1</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M70" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O70" s="10" t="n">
         <v>45384</v>
@@ -8497,7 +8503,7 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>35</v>
@@ -8530,13 +8536,13 @@
         <v>1</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O71" s="10" t="n">
         <v>45384</v>
@@ -8598,7 +8604,7 @@
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>35</v>
@@ -8631,13 +8637,13 @@
         <v>1</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M72" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O72" s="10" t="n">
         <v>45384</v>
@@ -8699,7 +8705,7 @@
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>35</v>
@@ -8732,13 +8738,13 @@
         <v>1</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O73" s="10" t="n">
         <v>45384</v>
@@ -8753,7 +8759,7 @@
         <v>7709577438</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T73" s="2" t="s">
         <v>39</v>
@@ -8800,7 +8806,7 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>35</v>
@@ -8833,13 +8839,13 @@
         <v>1</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="O74" s="10" t="n">
         <v>45384</v>
@@ -8854,7 +8860,7 @@
         <v>7709577438</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T74" s="2" t="s">
         <v>39</v>
@@ -8901,7 +8907,7 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>35</v>
@@ -8934,13 +8940,13 @@
         <v>1</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="O75" s="10" t="n">
         <v>45384</v>
@@ -8955,10 +8961,10 @@
         <v>7709577438</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="T75" s="20" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="U75" s="1" t="s">
         <v>39</v>
@@ -9002,7 +9008,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>35</v>
@@ -9035,13 +9041,13 @@
         <v>1</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="O76" s="10" t="n">
         <v>45384</v>
@@ -9056,10 +9062,10 @@
         <v>6060606060</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="T76" s="20" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="U76" s="1" t="s">
         <v>39</v>
@@ -9103,7 +9109,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>35</v>
@@ -9136,13 +9142,13 @@
         <v>1</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O77" s="10" t="n">
         <v>45384</v>
@@ -9157,10 +9163,10 @@
         <v>7070707070</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="T77" s="20" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="U77" s="1" t="s">
         <v>39</v>
@@ -9190,7 +9196,7 @@
         <v>39</v>
       </c>
       <c r="AD77" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AE77" s="8" t="s">
         <v>39</v>
@@ -9204,7 +9210,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>35</v>
@@ -9237,13 +9243,13 @@
         <v>1</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="O78" s="10" t="n">
         <v>45384</v>
@@ -9258,10 +9264,10 @@
         <v>7070707070</v>
       </c>
       <c r="S78" s="20" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="T78" s="20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U78" s="1" t="s">
         <v>39</v>
@@ -9305,7 +9311,7 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>35</v>
@@ -9338,13 +9344,13 @@
         <v>1</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O79" s="19" t="n">
         <v>45384</v>
@@ -9359,10 +9365,10 @@
         <v>2020202020</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U79" s="1" t="s">
         <v>39</v>
@@ -9386,13 +9392,13 @@
         <v>1</v>
       </c>
       <c r="AB79" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AC79" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AD79" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AE79" s="8" t="s">
         <v>39</v>
@@ -9406,7 +9412,7 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>35</v>
@@ -9439,13 +9445,13 @@
         <v>1</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="O80" s="10" t="n">
         <v>45384</v>
@@ -9460,7 +9466,7 @@
         <v>8080808080</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T80" s="2" t="s">
         <v>39</v>
@@ -9487,7 +9493,7 @@
         <v>1</v>
       </c>
       <c r="AB80" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AC80" s="8" t="s">
         <v>39</v>
@@ -9507,7 +9513,7 @@
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>35</v>
@@ -9540,13 +9546,13 @@
         <v>1</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="O81" s="10" t="n">
         <v>45384</v>
@@ -9561,7 +9567,7 @@
         <v>3030303030</v>
       </c>
       <c r="S81" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T81" s="2" t="s">
         <v>39</v>
@@ -9588,13 +9594,13 @@
         <v>1</v>
       </c>
       <c r="AB81" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AC81" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AD81" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AE81" s="8" t="s">
         <v>39</v>
@@ -9608,7 +9614,7 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>35</v>
@@ -9641,13 +9647,13 @@
         <v>1</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M82" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O82" s="10" t="n">
         <v>45384</v>
@@ -9705,10 +9711,10 @@
     </row>
     <row r="83" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>36</v>
@@ -9729,7 +9735,7 @@
         <v>600</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J83" s="9" t="n">
         <v>1</v>
@@ -9741,7 +9747,7 @@
         <v>39</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>39</v>
@@ -9762,7 +9768,7 @@
         <v>39</v>
       </c>
       <c r="T83" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="U83" s="4" t="s">
         <v>39</v>
@@ -9798,15 +9804,15 @@
         <v>39</v>
       </c>
       <c r="AF83" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>36</v>
@@ -9827,7 +9833,7 @@
         <v>600</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J84" s="9" t="n">
         <v>1</v>
@@ -9836,10 +9842,10 @@
         <v>1</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>39</v>
@@ -9857,7 +9863,7 @@
         <v>1111111101</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T84" s="2" t="s">
         <v>39</v>
@@ -9896,15 +9902,15 @@
         <v>39</v>
       </c>
       <c r="AF84" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>36</v>
@@ -9925,7 +9931,7 @@
         <v>600</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J85" s="9" t="n">
         <v>1</v>
@@ -9934,10 +9940,10 @@
         <v>1</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>39</v>
@@ -9955,7 +9961,7 @@
         <v>1111110101</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T85" s="2" t="s">
         <v>39</v>
@@ -9994,15 +10000,15 @@
         <v>39</v>
       </c>
       <c r="AF85" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" s="4" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>36</v>
@@ -10023,7 +10029,7 @@
         <v>600</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J86" s="9" t="n">
         <v>1</v>
@@ -10032,10 +10038,10 @@
         <v>1</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>39</v>
@@ -10053,7 +10059,7 @@
         <v>1111109101</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T86" s="2" t="s">
         <v>39</v>
@@ -10092,18 +10098,18 @@
         <v>39</v>
       </c>
       <c r="AF86" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AG86" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>36</v>
@@ -10124,7 +10130,7 @@
         <v>600</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J87" s="9" t="n">
         <v>1</v>
@@ -10133,10 +10139,10 @@
         <v>1</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>39</v>
@@ -10154,7 +10160,7 @@
         <v>1111108101</v>
       </c>
       <c r="S87" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T87" s="2" t="s">
         <v>39</v>
@@ -10193,15 +10199,15 @@
         <v>39</v>
       </c>
       <c r="AF87" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C88" s="13" t="s">
         <v>36</v>
@@ -10210,7 +10216,7 @@
         <v>123456</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F88" s="3" t="n">
         <v>123456</v>
@@ -10222,7 +10228,7 @@
         <v>600</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J88" s="9" t="n">
         <v>1</v>
@@ -10231,10 +10237,10 @@
         <v>1</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>39</v>
@@ -10252,7 +10258,7 @@
         <v>6000000000</v>
       </c>
       <c r="S88" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T88" s="2" t="s">
         <v>39</v>
@@ -10296,7 +10302,7 @@
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>35</v>
@@ -10394,7 +10400,7 @@
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>35</v>
@@ -10427,13 +10433,13 @@
         <v>1</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N90" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O90" s="10" t="n">
         <v>45384</v>
@@ -10460,10 +10466,10 @@
         <v>43</v>
       </c>
       <c r="W90" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X90" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="Y90" s="4" t="s">
         <v>55</v>
@@ -10492,7 +10498,7 @@
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>35</v>
@@ -10525,13 +10531,13 @@
         <v>1</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N91" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O91" s="10" t="n">
         <v>45384</v>
@@ -10558,7 +10564,7 @@
         <v>43</v>
       </c>
       <c r="W91" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X91" s="4" t="s">
         <v>44</v>
@@ -10590,7 +10596,7 @@
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>35</v>
@@ -10623,13 +10629,13 @@
         <v>1</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="O92" s="10" t="n">
         <v>45384</v>
@@ -10656,7 +10662,7 @@
         <v>43</v>
       </c>
       <c r="W92" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X92" s="4" t="s">
         <v>44</v>
@@ -10688,10 +10694,10 @@
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>36</v>
@@ -10789,10 +10795,10 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>36</v>
@@ -10890,10 +10896,10 @@
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>36</v>
@@ -10991,10 +10997,10 @@
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>36</v>
@@ -11003,7 +11009,7 @@
         <v>123456</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F96" s="3" t="n">
         <v>123456</v>
@@ -11092,10 +11098,10 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>36</v>
@@ -11167,7 +11173,7 @@
         <v>52</v>
       </c>
       <c r="Z97" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA97" s="5" t="s">
         <v>39</v>
@@ -11193,10 +11199,10 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>36</v>
@@ -11294,10 +11300,10 @@
     </row>
     <row r="99" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>36</v>
@@ -11392,10 +11398,10 @@
     </row>
     <row r="100" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>36</v>
@@ -11467,7 +11473,7 @@
         <v>52</v>
       </c>
       <c r="Z100" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AA100" s="5" t="s">
         <v>39</v>
@@ -11493,10 +11499,10 @@
     </row>
     <row r="101" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>36</v>
@@ -11568,7 +11574,7 @@
         <v>55</v>
       </c>
       <c r="Z101" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AA101" s="5" t="s">
         <v>39</v>
@@ -11594,10 +11600,10 @@
     </row>
     <row r="102" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>36</v>
@@ -11695,10 +11701,10 @@
     </row>
     <row r="103" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>36</v>
@@ -11796,10 +11802,10 @@
     </row>
     <row r="104" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>36</v>
@@ -11871,7 +11877,7 @@
         <v>59</v>
       </c>
       <c r="Z104" s="20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA104" s="5" t="s">
         <v>39</v>
@@ -11897,10 +11903,10 @@
     </row>
     <row r="105" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>36</v>
@@ -11972,7 +11978,7 @@
         <v>55</v>
       </c>
       <c r="Z105" s="20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA105" s="5" t="s">
         <v>39</v>
@@ -11998,10 +12004,10 @@
     </row>
     <row r="106" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>36</v>
@@ -12073,7 +12079,7 @@
         <v>52</v>
       </c>
       <c r="Z106" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AA106" s="5" t="s">
         <v>39</v>
@@ -12099,10 +12105,10 @@
     </row>
     <row r="107" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>36</v>
@@ -12174,7 +12180,7 @@
         <v>52</v>
       </c>
       <c r="Z107" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AA107" s="5" t="s">
         <v>39</v>
@@ -12200,10 +12206,10 @@
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>36</v>
@@ -12275,7 +12281,7 @@
         <v>52</v>
       </c>
       <c r="Z108" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA108" s="1" t="n">
         <v>1</v>
@@ -12301,10 +12307,10 @@
     </row>
     <row r="109" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>36</v>
@@ -12402,10 +12408,10 @@
     </row>
     <row r="110" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>36</v>
@@ -12503,10 +12509,10 @@
     </row>
     <row r="111" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="15" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>36</v>
@@ -12604,10 +12610,10 @@
     </row>
     <row r="112" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>36</v>
@@ -12705,10 +12711,10 @@
     </row>
     <row r="113" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>36</v>
@@ -12780,7 +12786,7 @@
         <v>52</v>
       </c>
       <c r="Z113" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA113" s="5" t="s">
         <v>39</v>
@@ -12806,10 +12812,10 @@
     </row>
     <row r="114" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>36</v>
@@ -12881,7 +12887,7 @@
         <v>52</v>
       </c>
       <c r="Z114" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA114" s="5" t="s">
         <v>39</v>
@@ -12907,10 +12913,10 @@
     </row>
     <row r="115" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>36</v>
@@ -12982,7 +12988,7 @@
         <v>52</v>
       </c>
       <c r="Z115" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA115" s="1" t="n">
         <v>0</v>
@@ -13008,10 +13014,10 @@
     </row>
     <row r="116" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>36</v>
@@ -13083,7 +13089,7 @@
         <v>52</v>
       </c>
       <c r="Z116" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA116" s="1" t="n">
         <v>1</v>
@@ -13109,10 +13115,10 @@
     </row>
     <row r="117" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>36</v>
@@ -13184,7 +13190,7 @@
         <v>52</v>
       </c>
       <c r="Z117" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA117" s="1" t="n">
         <v>1</v>
@@ -13210,10 +13216,10 @@
     </row>
     <row r="118" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>36</v>
@@ -13285,7 +13291,7 @@
         <v>52</v>
       </c>
       <c r="Z118" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA118" s="1" t="n">
         <v>1</v>
@@ -13311,10 +13317,10 @@
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>36</v>
@@ -13323,7 +13329,7 @@
         <v>123456</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F119" s="3" t="n">
         <v>123456</v>
@@ -13386,7 +13392,7 @@
         <v>52</v>
       </c>
       <c r="Z119" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA119" s="1" t="n">
         <v>1</v>
@@ -13412,10 +13418,10 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>36</v>
@@ -13487,7 +13493,7 @@
         <v>52</v>
       </c>
       <c r="Z120" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA120" s="1" t="n">
         <v>1</v>
@@ -13513,10 +13519,10 @@
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>36</v>
@@ -13588,7 +13594,7 @@
         <v>52</v>
       </c>
       <c r="Z121" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA121" s="1" t="n">
         <v>1</v>
@@ -13614,10 +13620,10 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>36</v>
@@ -13689,7 +13695,7 @@
         <v>52</v>
       </c>
       <c r="Z122" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA122" s="1" t="n">
         <v>1</v>
@@ -13715,10 +13721,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>36</v>
@@ -13790,7 +13796,7 @@
         <v>52</v>
       </c>
       <c r="Z123" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA123" s="1" t="n">
         <v>1</v>
@@ -13816,10 +13822,10 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>36</v>
@@ -13891,7 +13897,7 @@
         <v>52</v>
       </c>
       <c r="Z124" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA124" s="1" t="n">
         <v>1</v>
@@ -13906,7 +13912,7 @@
         <v>39</v>
       </c>
       <c r="AE124" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AF124" s="8" t="s">
         <v>39</v>
@@ -13917,10 +13923,10 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>36</v>
@@ -13992,7 +13998,7 @@
         <v>52</v>
       </c>
       <c r="Z125" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA125" s="1" t="n">
         <v>1</v>
@@ -14007,7 +14013,7 @@
         <v>39</v>
       </c>
       <c r="AE125" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AF125" s="8" t="s">
         <v>39</v>
@@ -14018,10 +14024,10 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>36</v>
@@ -14093,7 +14099,7 @@
         <v>52</v>
       </c>
       <c r="Z126" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA126" s="1" t="n">
         <v>1</v>
@@ -14108,7 +14114,7 @@
         <v>39</v>
       </c>
       <c r="AE126" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AF126" s="8" t="s">
         <v>39</v>
@@ -14119,10 +14125,10 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>36</v>
@@ -14194,7 +14200,7 @@
         <v>52</v>
       </c>
       <c r="Z127" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA127" s="1" t="n">
         <v>1</v>
@@ -14209,7 +14215,7 @@
         <v>39</v>
       </c>
       <c r="AE127" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF127" s="8" t="s">
         <v>39</v>
@@ -14220,10 +14226,10 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>36</v>
@@ -14295,7 +14301,7 @@
         <v>52</v>
       </c>
       <c r="Z128" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA128" s="1" t="n">
         <v>1</v>
@@ -14310,7 +14316,7 @@
         <v>39</v>
       </c>
       <c r="AE128" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF128" s="8" t="s">
         <v>39</v>
@@ -14321,10 +14327,10 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>36</v>
@@ -14396,7 +14402,7 @@
         <v>52</v>
       </c>
       <c r="Z129" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA129" s="1" t="n">
         <v>1</v>
@@ -14411,7 +14417,7 @@
         <v>39</v>
       </c>
       <c r="AE129" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF129" s="8" t="s">
         <v>39</v>
@@ -14422,10 +14428,10 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>36</v>
@@ -14497,7 +14503,7 @@
         <v>52</v>
       </c>
       <c r="Z130" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA130" s="1" t="n">
         <v>1</v>
@@ -14512,7 +14518,7 @@
         <v>39</v>
       </c>
       <c r="AE130" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AF130" s="8" t="s">
         <v>39</v>
@@ -14523,10 +14529,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>36</v>
@@ -14598,7 +14604,7 @@
         <v>52</v>
       </c>
       <c r="Z131" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA131" s="1" t="n">
         <v>1</v>
@@ -14613,7 +14619,7 @@
         <v>39</v>
       </c>
       <c r="AE131" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AF131" s="8" t="s">
         <v>39</v>
@@ -14624,10 +14630,10 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>36</v>
@@ -14699,7 +14705,7 @@
         <v>52</v>
       </c>
       <c r="Z132" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AA132" s="1" t="n">
         <v>1</v>
@@ -14711,7 +14717,7 @@
         <v>39</v>
       </c>
       <c r="AE132" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AF132" s="8" t="s">
         <v>39</v>
@@ -14722,82 +14728,82 @@
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>